<commit_message>
AE-365 implement swedish mappings for 2018 energiatodistus
</commit_message>
<xml_diff>
--- a/etp-backend/src/main/resources/energiatodistus-2018-sv.xlsx
+++ b/etp-backend/src/main/resources/energiatodistus-2018-sv.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="1) etusivu" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,23 +19,23 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'1) etusivu'!$A$1:$Q$51</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$59</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$58</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area" vbProcedure="false">'3) E-luvun laskennan lähtöt.'!$B$2:$G$67</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$1:$G$78</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$2:$G$77</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area" vbProcedure="false">'5) toteutunut kulutus'!$B$2:$J$55</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm.Print_Area" vbProcedure="false">'6) huomiot 1'!$B$2:$F$53</definedName>
-    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$61</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$60</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area" vbProcedure="false">'8) lisämerkintöjä'!$B$2:$H$63</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'1) etusivu'!$A$1:$Q$50</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'2) E-luokka'!$B$2:$K$59</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$58</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$59</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'3) E-luvun laskennan lähtöt.'!$B$2:$G$66</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$2:$G$76</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$2:$G$77</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$1:$G$78</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'5) toteutunut kulutus'!$B$2:$K$54</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'6) huomiot 1'!$B$2:$G$52</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'7) huomiot 2'!$B$2:$G$59</definedName>
-    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$60</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$61</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'8) lisämerkintöjä'!$B$2:$I$62</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -2338,7 +2338,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="6" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -6211,9 +6211,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>238680</xdr:colOff>
+      <xdr:colOff>238320</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>253080</xdr:rowOff>
+      <xdr:rowOff>252720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6227,7 +6227,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="4656960"/>
-          <a:ext cx="748800" cy="205560"/>
+          <a:ext cx="748440" cy="205200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6248,9 +6248,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>138600</xdr:colOff>
+      <xdr:colOff>138240</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>253080</xdr:rowOff>
+      <xdr:rowOff>252720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6264,7 +6264,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="4971240"/>
-          <a:ext cx="1092240" cy="205560"/>
+          <a:ext cx="1091880" cy="205200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6285,9 +6285,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>11880</xdr:colOff>
+      <xdr:colOff>11520</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>253080</xdr:rowOff>
+      <xdr:rowOff>252720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6301,7 +6301,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="5285520"/>
-          <a:ext cx="1398960" cy="205560"/>
+          <a:ext cx="1398600" cy="205200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6322,9 +6322,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>335880</xdr:colOff>
+      <xdr:colOff>335520</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>253080</xdr:rowOff>
+      <xdr:rowOff>252720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6338,7 +6338,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="5599800"/>
-          <a:ext cx="1722960" cy="205560"/>
+          <a:ext cx="1722600" cy="205200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6359,9 +6359,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>209160</xdr:colOff>
+      <xdr:colOff>208800</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>266040</xdr:rowOff>
+      <xdr:rowOff>265680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6375,7 +6375,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="5909760"/>
-          <a:ext cx="2030040" cy="218520"/>
+          <a:ext cx="2029680" cy="218160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6396,9 +6396,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>152280</xdr:colOff>
+      <xdr:colOff>151920</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>253080</xdr:rowOff>
+      <xdr:rowOff>252720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6412,7 +6412,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="6219720"/>
-          <a:ext cx="2366280" cy="205560"/>
+          <a:ext cx="2365920" cy="205200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6433,9 +6433,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>92520</xdr:colOff>
+      <xdr:colOff>92160</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>253080</xdr:rowOff>
+      <xdr:rowOff>252720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6445,7 +6445,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="6530400"/>
-          <a:ext cx="2679120" cy="204480"/>
+          <a:ext cx="2678760" cy="204120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6814,9 +6814,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>291960</xdr:colOff>
+      <xdr:colOff>291600</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>92520</xdr:rowOff>
+      <xdr:rowOff>92160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6826,7 +6826,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="149400" y="78480"/>
-          <a:ext cx="6978240" cy="10548000"/>
+          <a:ext cx="6977880" cy="10547640"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6955,8 +6955,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P27" activeCellId="0" sqref="P27"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8497,8 +8497,8 @@
   </sheetPr>
   <dimension ref="B1:AA65"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C58" activeCellId="0" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15033,8 +15033,8 @@
   </sheetPr>
   <dimension ref="B1:G60"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B60" activeCellId="0" sqref="B60"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F52" activeCellId="0" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15619,9 +15619,6 @@
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="B54" r:id="rId1" display="Motiva Oy - Sakkunnig i effektiv användning av energi och material, www.motiva.fi"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
AE-553 update last page of xlsx templates
</commit_message>
<xml_diff>
--- a/etp-backend/src/main/resources/energiatodistus-2018-sv.xlsx
+++ b/etp-backend/src/main/resources/energiatodistus-2018-sv.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="1) etusivu" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,24 +19,23 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'1) etusivu'!$B$1:$R$51</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$58</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$59</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area" vbProcedure="false">'3) E-luvun laskennan lähtöt.'!$B$2:$G$67</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$2:$G$77</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$1:$G$78</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area" vbProcedure="false">'5) toteutunut kulutus'!$B$2:$K$55</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm.Print_Area" vbProcedure="false">'6) huomiot 1'!$B$2:$F$53</definedName>
-    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$60</definedName>
-    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area" vbProcedure="false">'8) lisämerkintöjä'!$B$2:$H$63</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$61</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area" vbProcedure="false">'8) lisämerkintöjä'!$B$1:$M$63</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'1) etusivu'!$B$1:$R$50</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'2) E-luokka'!$B$2:$K$59</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$59</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$58</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'3) E-luvun laskennan lähtöt.'!$B$2:$G$66</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$2:$G$76</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$1:$G$78</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$2:$G$77</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'5) toteutunut kulutus'!$B$2:$L$54</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'6) huomiot 1'!$B$2:$G$52</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'7) huomiot 2'!$B$2:$G$59</definedName>
-    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$61</definedName>
-    <definedName function="false" hidden="false" localSheetId="7" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'8) lisämerkintöjä'!$B$2:$I$62</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$60</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -48,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="747">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="777">
   <si>
     <t xml:space="preserve">[:id]</t>
   </si>
@@ -1606,16 +1605,16 @@
     <t xml:space="preserve">[:tulokset :kaytettavat-energiamuodot :uusiutuva-polttoaine-kertoimella]</t>
   </si>
   <si>
-    <t xml:space="preserve">TODO aurinkosähkö</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TODO aurinkolämpö</t>
+    <t xml:space="preserve">Solel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solvärme</t>
   </si>
   <si>
     <t xml:space="preserve">[:tulokset :kaytettavat-energiamuodot :muu 0 :ostoenergia-kertoimella]</t>
   </si>
   <si>
-    <t xml:space="preserve">TODO tuulisähkö</t>
+    <t xml:space="preserve">Vindel</t>
   </si>
   <si>
     <t xml:space="preserve">TODO Lämpöpumpun lämmönlähteestä ottama energia</t>
@@ -2786,12 +2785,12 @@
     <t xml:space="preserve">[:tulokset :kuukausierittely 0 :tuotto :aurinkolampo]</t>
   </si>
   <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 0 :tuotto :lampopumppu]</t>
+  </si>
+  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 0 :tuotto :muulampo]</t>
   </si>
   <si>
-    <t xml:space="preserve">[:tulokset :kuukausierittely 0 :tuotto :lampopumppu]</t>
-  </si>
-  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 0 :kulutus :sahko]</t>
   </si>
   <si>
@@ -2816,12 +2815,12 @@
     <t xml:space="preserve">[:tulokset :kuukausierittely 1 :tuotto :aurinkolampo]</t>
   </si>
   <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 1 :tuotto :lampopumppu]</t>
+  </si>
+  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 1 :tuotto :muulampo]</t>
   </si>
   <si>
-    <t xml:space="preserve">[:tulokset :kuukausierittely 1 :tuotto :lampopumppu]</t>
-  </si>
-  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 1 :kulutus :sahko]</t>
   </si>
   <si>
@@ -2846,87 +2845,404 @@
     <t xml:space="preserve">[:tulokset :kuukausierittely 2 :tuotto :aurinkolampo]</t>
   </si>
   <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 2 :tuotto :lampopumppu]</t>
+  </si>
+  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 2 :tuotto :muulampo]</t>
   </si>
   <si>
-    <t xml:space="preserve">[:tulokset :kuukausierittely 2 :tuotto :lampopumppu]</t>
+    <t xml:space="preserve">Kuukausitason erittely ympäristöstä olevasta energiasta otetun energian määrästä</t>
   </si>
   <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 2 :kulutus :sahko]</t>
   </si>
   <si>
+    <t xml:space="preserve">Sähköenergiantuotto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lämpöenergiantuotto</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF009EE0"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Energiankulutus</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF009EE0"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Hyödynnetty osuus</t>
+  </si>
+  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 2 :kulutus :lampo]</t>
   </si>
   <si>
+    <t xml:space="preserve">Månad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kWh/kk</t>
+  </si>
+  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 2 :hyoty :sahko]</t>
   </si>
   <si>
+    <t xml:space="preserve">Muu sähkö</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lämpöpumppu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muu lämpö</t>
+  </si>
+  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 2 :hyoty :lampo]</t>
   </si>
   <si>
+    <t xml:space="preserve">Januari</t>
+  </si>
+  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 3 :tuotto :aurinkosahko]</t>
   </si>
   <si>
+    <t xml:space="preserve">Februari</t>
+  </si>
+  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 3 :tuotto :tuulisahko]</t>
   </si>
   <si>
+    <t xml:space="preserve">Mars</t>
+  </si>
+  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 3 :tuotto :muusahko]</t>
   </si>
   <si>
+    <t xml:space="preserve">April</t>
+  </si>
+  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 3 :tuotto :aurinkolampo]</t>
   </si>
   <si>
+    <t xml:space="preserve">Maj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 3 :tuotto :lampopumppu]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juni</t>
+  </si>
+  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 3 :tuotto :muulampo]</t>
   </si>
   <si>
-    <t xml:space="preserve">[:tulokset :kuukausierittely 3 :tuotto :lampopumppu]</t>
+    <t xml:space="preserve">Juli</t>
   </si>
   <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 3 :kulutus :sahko]</t>
   </si>
   <si>
+    <t xml:space="preserve">Augusti</t>
+  </si>
+  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 3 :kulutus :lampo]</t>
   </si>
   <si>
+    <t xml:space="preserve">September</t>
+  </si>
+  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 3 :hyoty :sahko]</t>
   </si>
   <si>
+    <t xml:space="preserve">Oktober</t>
+  </si>
+  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 3 :hyoty :lampo]</t>
   </si>
   <si>
+    <t xml:space="preserve">November</t>
+  </si>
+  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 4 :tuotto :aurinkosahko]</t>
   </si>
   <si>
+    <t xml:space="preserve">December</t>
+  </si>
+  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 4 :tuotto :tuulisahko]</t>
   </si>
   <si>
+    <t xml:space="preserve">Totalt</t>
+  </si>
+  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 4 :tuotto :muusahko]</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="7.5"/>
+        <color rgb="FF009EE0"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7.5"/>
+        <color rgb="FF009EE0"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Energiankulutukseen merkitään se osuus rakennuksen energiankulutuksesta, jonka määrää voidaan vähentää ympäristössä olevasta energiasta otetulla energialla.</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 4 :tuotto :aurinkolampo]</t>
   </si>
   <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 4 :tuotto :lampopumppu]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energiatodistuksen laatimisessa käytettyjä lähtötietoja</t>
+  </si>
+  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 4 :tuotto :muulampo]</t>
   </si>
   <si>
-    <t xml:space="preserve">[:tulokset :kuukausierittely 4 :tuotto :lampopumppu]</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF009EE0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Lämpökapasiteetti Crak ominaisarvo C </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color rgb="FF009EE0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">rak omin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF009EE0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, Wh/m²K</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 4 :kulutus :sahko]</t>
   </si>
   <si>
+    <t xml:space="preserve">Rakennuksen ilmatilavuus V, m³</t>
+  </si>
+  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 4 :kulutus :lampo]</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF009EE0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Tuloilman sisäänpuhalluslämpötila T</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color rgb="FF009EE0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">sp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF009EE0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, °C</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 4 :hyoty :sahko]</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF009EE0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Lämpöpumpun tuotto-osuus tilojen lämpöenergian tarpeesta Q</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color rgb="FF009EE0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">LP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF009EE0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/Q</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color rgb="FF009EE0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">lämmitys, tilat</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF009EE0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 4 :hyoty :lampo]</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF009EE0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Lämpöpumpun tuotto-osuus käyttöveden lämpöenergian tarpeesta Q</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color rgb="FF009EE0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">LP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF009EE0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/Q</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color rgb="FF009EE0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">lämmitys, lkv</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 5 :tuotto :aurinkosahko]</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF009EE0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Lämmönjakelujärjestelmän lämpöhäviöt lämmittämättömään tilaan Q</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color rgb="FF009EE0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">jakelu, ulos</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF009EE0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, kWh/a</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 5 :tuotto :tuulisahko]</t>
   </si>
   <si>
@@ -2936,12 +3252,12 @@
     <t xml:space="preserve">[:tulokset :kuukausierittely 5 :tuotto :aurinkolampo]</t>
   </si>
   <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 5 :tuotto :lampopumppu]</t>
+  </si>
+  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 5 :tuotto :muulampo]</t>
   </si>
   <si>
-    <t xml:space="preserve">[:tulokset :kuukausierittely 5 :tuotto :lampopumppu]</t>
-  </si>
-  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 5 :kulutus :sahko]</t>
   </si>
   <si>
@@ -2966,12 +3282,12 @@
     <t xml:space="preserve">[:tulokset :kuukausierittely 6 :tuotto :aurinkolampo]</t>
   </si>
   <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 6 :tuotto :lampopumppu]</t>
+  </si>
+  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 6 :tuotto :muulampo]</t>
   </si>
   <si>
-    <t xml:space="preserve">[:tulokset :kuukausierittely 6 :tuotto :lampopumppu]</t>
-  </si>
-  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 6 :kulutus :sahko]</t>
   </si>
   <si>
@@ -2996,12 +3312,12 @@
     <t xml:space="preserve">[:tulokset :kuukausierittely 7 :tuotto :aurinkolampo]</t>
   </si>
   <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 7 :tuotto :lampopumppu]</t>
+  </si>
+  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 7 :tuotto :muulampo]</t>
   </si>
   <si>
-    <t xml:space="preserve">[:tulokset :kuukausierittely 7 :tuotto :lampopumppu]</t>
-  </si>
-  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 7 :kulutus :sahko]</t>
   </si>
   <si>
@@ -3026,12 +3342,12 @@
     <t xml:space="preserve">[:tulokset :kuukausierittely 8 :tuotto :aurinkolampo]</t>
   </si>
   <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 8 :tuotto :lampopumppu]</t>
+  </si>
+  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 8 :tuotto :muulampo]</t>
   </si>
   <si>
-    <t xml:space="preserve">[:tulokset :kuukausierittely 8 :tuotto :lampopumppu]</t>
-  </si>
-  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 8 :kulutus :sahko]</t>
   </si>
   <si>
@@ -3056,12 +3372,12 @@
     <t xml:space="preserve">[:tulokset :kuukausierittely 9 :tuotto :aurinkolampo]</t>
   </si>
   <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 9 :tuotto :lampopumppu]</t>
+  </si>
+  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 9 :tuotto :muulampo]</t>
   </si>
   <si>
-    <t xml:space="preserve">[:tulokset :kuukausierittely 9 :tuotto :lampopumppu]</t>
-  </si>
-  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 9 :kulutus :sahko]</t>
   </si>
   <si>
@@ -3086,12 +3402,12 @@
     <t xml:space="preserve">[:tulokset :kuukausierittely 10 :tuotto :aurinkolampo]</t>
   </si>
   <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 10 :tuotto :lampopumppu]</t>
+  </si>
+  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 10 :tuotto :muulampo]</t>
   </si>
   <si>
-    <t xml:space="preserve">[:tulokset :kuukausierittely 10 :tuotto :lampopumppu]</t>
-  </si>
-  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 10 :kulutus :sahko]</t>
   </si>
   <si>
@@ -3116,12 +3432,12 @@
     <t xml:space="preserve">[:tulokset :kuukausierittely 11 :tuotto :aurinkolampo]</t>
   </si>
   <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 11 :tuotto :lampopumppu]</t>
+  </si>
+  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 11 :tuotto :muulampo]</t>
   </si>
   <si>
-    <t xml:space="preserve">[:tulokset :kuukausierittely 11 :tuotto :lampopumppu]</t>
-  </si>
-  <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 11 :kulutus :sahko]</t>
   </si>
   <si>
@@ -3134,34 +3450,31 @@
     <t xml:space="preserve">[:tulokset :kuukausierittely 11 :hyoty :lampo]</t>
   </si>
   <si>
-    <t xml:space="preserve">[:tulokset :kuukausierittely 12 :tuotto :aurinkosahko]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[:tulokset :kuukausierittely 12 :tuotto :tuulisahko]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[:tulokset :kuukausierittely 12 :tuotto :muusahko]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[:tulokset :kuukausierittely 12 :tuotto :aurinkolampo]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[:tulokset :kuukausierittely 12 :tuotto :muulampo]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[:tulokset :kuukausierittely 12 :tuotto :lampopumppu]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[:tulokset :kuukausierittely 12 :kulutus :sahko]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[:tulokset :kuukausierittely 12 :kulutus :lampo]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[:tulokset :kuukausierittely 12 :hyoty :sahko]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[:tulokset :kuukausierittely 12 :hyoty :lampo]</t>
+    <t xml:space="preserve">[:tulokset :kuukausierittely-summat :tuotto :aurinkosahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely-summat :tuotto :tuulisahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely-summat :tuotto :muulampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely-summat :tuotto :aurinkolampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely-summat :tuotto :lampopumppu]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely-summat :kulutus :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely-summat :kulutus :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely-summat :hyoty :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely-summat :hyoty :lampo]</t>
   </si>
 </sst>
 </file>
@@ -3181,7 +3494,7 @@
     <numFmt numFmtId="173" formatCode="0%"/>
     <numFmt numFmtId="174" formatCode="0"/>
   </numFmts>
-  <fonts count="45">
+  <fonts count="55">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -3514,6 +3827,81 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF009EE0"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <color rgb="FF009EE0"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF009EE0"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="7.5"/>
+      <color rgb="FF009EE0"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="7.5"/>
+      <color rgb="FF009EE0"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF009EE0"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -3806,7 +4194,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="394">
+  <cellXfs count="430">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3943,7 +4331,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -5375,11 +5763,155 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="36" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="45" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="46" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="47" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="47" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="48" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="48" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="48" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="50" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="50" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="50" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="50" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="50" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="50" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="48" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="51" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="53" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="54" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -7677,6 +8209,11 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="0"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF99"/>
@@ -7758,9 +8295,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>232560</xdr:colOff>
+      <xdr:colOff>232200</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>246960</xdr:rowOff>
+      <xdr:rowOff>246600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7774,7 +8311,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="4656960"/>
-          <a:ext cx="742680" cy="199440"/>
+          <a:ext cx="742320" cy="199080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7795,9 +8332,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>132480</xdr:colOff>
+      <xdr:colOff>132120</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>246960</xdr:rowOff>
+      <xdr:rowOff>246600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7811,7 +8348,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="4971240"/>
-          <a:ext cx="1086120" cy="199440"/>
+          <a:ext cx="1085760" cy="199080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7832,9 +8369,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>5760</xdr:colOff>
+      <xdr:colOff>5400</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>246960</xdr:rowOff>
+      <xdr:rowOff>246600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7848,7 +8385,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="5285520"/>
-          <a:ext cx="1392840" cy="199440"/>
+          <a:ext cx="1392480" cy="199080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7869,9 +8406,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>329760</xdr:colOff>
+      <xdr:colOff>329400</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>246960</xdr:rowOff>
+      <xdr:rowOff>246600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7885,7 +8422,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="5599800"/>
-          <a:ext cx="1716840" cy="199440"/>
+          <a:ext cx="1716480" cy="199080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7906,9 +8443,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>203040</xdr:colOff>
+      <xdr:colOff>202680</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>259920</xdr:rowOff>
+      <xdr:rowOff>259560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7922,7 +8459,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="5909760"/>
-          <a:ext cx="2023920" cy="212400"/>
+          <a:ext cx="2023560" cy="212040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7943,9 +8480,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>146160</xdr:colOff>
+      <xdr:colOff>145800</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>246960</xdr:rowOff>
+      <xdr:rowOff>246600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7959,7 +8496,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="6219720"/>
-          <a:ext cx="2360160" cy="199440"/>
+          <a:ext cx="2359800" cy="199080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7980,9 +8517,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>86400</xdr:colOff>
+      <xdr:colOff>86040</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>248040</xdr:rowOff>
+      <xdr:rowOff>247680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7992,7 +8529,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="6531480"/>
-          <a:ext cx="2673000" cy="198360"/>
+          <a:ext cx="2672640" cy="198000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8361,9 +8898,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>285840</xdr:colOff>
+      <xdr:colOff>285480</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>87120</xdr:rowOff>
+      <xdr:rowOff>86760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -8373,7 +8910,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1978200" y="78480"/>
-          <a:ext cx="6972120" cy="10493640"/>
+          <a:ext cx="6971760" cy="10493280"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -8502,7 +9039,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G7" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G7" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J18" activeCellId="0" sqref="J18"/>
     </sheetView>
   </sheetViews>
@@ -12355,7 +12892,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ92"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G42" activeCellId="0" sqref="G42"/>
     </sheetView>
   </sheetViews>
@@ -14223,63 +14760,63 @@
   </conditionalFormatting>
   <dataValidations count="15">
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E4" type="custom">
-      <formula1>OR(ISNUMBER(B50),B50="*")</formula1>
+      <formula1>OR(ISNUMBER(#REF!),#REF!="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E10" type="none">
-      <formula1>OR(ISNUMBER(E12),E12="*")</formula1>
+      <formula1>OR(ISNUMBER(#REF!),#REF!="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E11 E13:E14" type="none">
-      <formula1>OR(ISNUMBER(E13),E13="*")</formula1>
+      <formula1>OR(ISNUMBER(#REF!),#REF!="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F15" type="none">
-      <formula1>OR(ISNUMBER(F17),F17="*")</formula1>
+      <formula1>OR(ISNUMBER(#REF!),#REF!="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G15" type="none">
-      <formula1>OR(ISNUMBER(G17),G17="*")</formula1>
+      <formula1>OR(ISNUMBER(#REF!),#REF!="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D19:D21 E20 D22:D26" type="none">
-      <formula1>OR(ISNUMBER(D21),D21="*")</formula1>
+      <formula1>OR(ISNUMBER(#REF!),#REF!="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E19:F19 F20:F26 E21:E26" type="none">
-      <formula1>OR(ISNUMBER(E21),E21="*")</formula1>
+      <formula1>OR(ISNUMBER(#REF!),#REF!="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D33:F33" type="none">
-      <formula1>OR(ISNUMBER(E35),E35="*")</formula1>
+      <formula1>OR(ISNUMBER(#REF!),#REF!="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D34:E34" type="none">
-      <formula1>OR(ISNUMBER(E36),E36="*")</formula1>
+      <formula1>OR(ISNUMBER(#REF!),#REF!="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D35:E35" type="none">
-      <formula1>OR(ISNUMBER(E37),E37="*")</formula1>
+      <formula1>OR(ISNUMBER(#REF!),#REF!="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G33" type="none">
-      <formula1>OR(ISNUMBER(G35),G35="*")</formula1>
+      <formula1>OR(ISNUMBER(#REF!),#REF!="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E36" type="none">
-      <formula1>OR(ISNUMBER(E38),E38="*")</formula1>
+      <formula1>OR(ISNUMBER(#REF!),#REF!="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D43:G44" type="none">
-      <formula1>OR(ISNUMBER(D7),D7="*")</formula1>
+      <formula1>OR(ISNUMBER(#REF!),#REF!="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D50:E51" type="none">
-      <formula1>OR(ISNUMBER(D14),D14="*")</formula1>
+      <formula1>OR(ISNUMBER(#REF!),#REF!="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D55:E55 D59:E59 D63:G65" type="none">
-      <formula1>OR(ISNUMBER(D27),D27="*")</formula1>
+      <formula1>OR(ISNUMBER(#REF!),#REF!="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -14300,8 +14837,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ113"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14782,7 +15319,7 @@
       <c r="F27" s="195"/>
       <c r="G27" s="203"/>
     </row>
-    <row r="28" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="166" t="s">
         <v>86</v>
       </c>
@@ -14801,7 +15338,7 @@
       </c>
       <c r="G28" s="279"/>
     </row>
-    <row r="29" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="166" t="s">
         <v>89</v>
       </c>
@@ -14820,7 +15357,7 @@
       </c>
       <c r="G29" s="279"/>
     </row>
-    <row r="30" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="166" t="s">
         <v>298</v>
       </c>
@@ -16202,8 +16739,8 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="97" width="49.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="98" width="1.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="98" width="18.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="98" width="7.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="98" width="18.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="98" width="7.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="5" style="98" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="98" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="98" width="2.31"/>
@@ -18920,8 +19457,8 @@
   </sheetPr>
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B55" activeCellId="0" sqref="B55"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B59" activeCellId="0" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19773,20 +20310,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:I140"/>
+  <dimension ref="A1:Q140"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A48" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C90" activeCellId="0" sqref="C90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="366" width="25.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="5.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="3" style="3" width="15.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="1.12"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="994" min="10" style="3" width="9.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="995" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="366" width="27.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="1.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="9.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="4" style="3" width="10.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="3" width="1.12"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="999" min="15" style="3" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1000" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="7.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19794,1163 +20332,1978 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="166" t="s">
         <v>607</v>
       </c>
-      <c r="B2" s="392" t="s">
+      <c r="B2" s="392"/>
+      <c r="C2" s="393" t="s">
         <v>608</v>
       </c>
-      <c r="C2" s="392"/>
-      <c r="D2" s="392"/>
-      <c r="E2" s="392"/>
-      <c r="F2" s="392"/>
-      <c r="G2" s="392"/>
-      <c r="H2" s="392"/>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D2" s="393"/>
+      <c r="E2" s="393"/>
+      <c r="F2" s="393"/>
+      <c r="G2" s="393"/>
+      <c r="H2" s="393"/>
+      <c r="I2" s="393"/>
+      <c r="J2" s="393"/>
+      <c r="K2" s="393"/>
+      <c r="L2" s="393"/>
+      <c r="M2" s="393"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="366" t="s">
         <v>609</v>
       </c>
-      <c r="B3" s="373" t="str">
+      <c r="B3" s="357"/>
+      <c r="C3" s="394" t="str">
         <f aca="false">A3</f>
         <v>[:lisamerkintoja-sv]</v>
       </c>
-      <c r="C3" s="373"/>
-      <c r="D3" s="373"/>
-      <c r="E3" s="373"/>
-      <c r="F3" s="373"/>
-      <c r="G3" s="373"/>
-      <c r="H3" s="373"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D3" s="394"/>
+      <c r="E3" s="394"/>
+      <c r="F3" s="394"/>
+      <c r="G3" s="394"/>
+      <c r="H3" s="394"/>
+      <c r="I3" s="394"/>
+      <c r="J3" s="394"/>
+      <c r="K3" s="394"/>
+      <c r="L3" s="394"/>
+      <c r="M3" s="394"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="366" t="s">
         <v>610</v>
       </c>
-      <c r="B4" s="373"/>
-      <c r="C4" s="373"/>
-      <c r="D4" s="373"/>
-      <c r="E4" s="373"/>
-      <c r="F4" s="373"/>
-      <c r="G4" s="373"/>
-      <c r="H4" s="373"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="357"/>
+      <c r="C4" s="394"/>
+      <c r="D4" s="394"/>
+      <c r="E4" s="394"/>
+      <c r="F4" s="394"/>
+      <c r="G4" s="394"/>
+      <c r="H4" s="394"/>
+      <c r="I4" s="394"/>
+      <c r="J4" s="394"/>
+      <c r="K4" s="394"/>
+      <c r="L4" s="394"/>
+      <c r="M4" s="394"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="366" t="s">
         <v>611</v>
       </c>
-      <c r="B5" s="373"/>
-      <c r="C5" s="373"/>
-      <c r="D5" s="373"/>
-      <c r="E5" s="373"/>
-      <c r="F5" s="373"/>
-      <c r="G5" s="373"/>
-      <c r="H5" s="373"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="357"/>
+      <c r="C5" s="394"/>
+      <c r="D5" s="394"/>
+      <c r="E5" s="394"/>
+      <c r="F5" s="394"/>
+      <c r="G5" s="394"/>
+      <c r="H5" s="394"/>
+      <c r="I5" s="394"/>
+      <c r="J5" s="394"/>
+      <c r="K5" s="394"/>
+      <c r="L5" s="394"/>
+      <c r="M5" s="394"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="366" t="s">
         <v>612</v>
       </c>
-      <c r="B6" s="373"/>
-      <c r="C6" s="373"/>
-      <c r="D6" s="373"/>
-      <c r="E6" s="373"/>
-      <c r="F6" s="373"/>
-      <c r="G6" s="373"/>
-      <c r="H6" s="373"/>
-      <c r="I6" s="4"/>
-    </row>
-    <row r="7" customFormat="false" ht="7.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B6" s="357"/>
+      <c r="C6" s="394"/>
+      <c r="D6" s="394"/>
+      <c r="E6" s="394"/>
+      <c r="F6" s="394"/>
+      <c r="G6" s="394"/>
+      <c r="H6" s="394"/>
+      <c r="I6" s="394"/>
+      <c r="J6" s="394"/>
+      <c r="K6" s="394"/>
+      <c r="L6" s="394"/>
+      <c r="M6" s="394"/>
+      <c r="N6" s="4"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="366" t="s">
         <v>613</v>
       </c>
-      <c r="B7" s="373"/>
-      <c r="C7" s="373"/>
-      <c r="D7" s="373"/>
-      <c r="E7" s="373"/>
-      <c r="F7" s="373"/>
-      <c r="G7" s="373"/>
-      <c r="H7" s="373"/>
-      <c r="I7" s="13"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="357"/>
+      <c r="C7" s="394"/>
+      <c r="D7" s="394"/>
+      <c r="E7" s="394"/>
+      <c r="F7" s="394"/>
+      <c r="G7" s="394"/>
+      <c r="H7" s="394"/>
+      <c r="I7" s="394"/>
+      <c r="J7" s="394"/>
+      <c r="K7" s="394"/>
+      <c r="L7" s="394"/>
+      <c r="M7" s="394"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="231"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="366" t="s">
         <v>614</v>
       </c>
-      <c r="B8" s="373"/>
-      <c r="C8" s="373"/>
-      <c r="D8" s="373"/>
-      <c r="E8" s="373"/>
-      <c r="F8" s="373"/>
-      <c r="G8" s="373"/>
-      <c r="H8" s="373"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="357"/>
+      <c r="C8" s="394"/>
+      <c r="D8" s="394"/>
+      <c r="E8" s="394"/>
+      <c r="F8" s="394"/>
+      <c r="G8" s="394"/>
+      <c r="H8" s="394"/>
+      <c r="I8" s="394"/>
+      <c r="J8" s="394"/>
+      <c r="K8" s="394"/>
+      <c r="L8" s="394"/>
+      <c r="M8" s="394"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="366" t="s">
         <v>615</v>
       </c>
-      <c r="B9" s="373"/>
-      <c r="C9" s="373"/>
-      <c r="D9" s="373"/>
-      <c r="E9" s="373"/>
-      <c r="F9" s="373"/>
-      <c r="G9" s="373"/>
-      <c r="H9" s="373"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="357"/>
+      <c r="C9" s="394"/>
+      <c r="D9" s="394"/>
+      <c r="E9" s="394"/>
+      <c r="F9" s="394"/>
+      <c r="G9" s="394"/>
+      <c r="H9" s="394"/>
+      <c r="I9" s="394"/>
+      <c r="J9" s="394"/>
+      <c r="K9" s="394"/>
+      <c r="L9" s="394"/>
+      <c r="M9" s="394"/>
+      <c r="P9" s="231"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="366" t="s">
         <v>616</v>
       </c>
-      <c r="B10" s="373"/>
-      <c r="C10" s="373"/>
-      <c r="D10" s="373"/>
-      <c r="E10" s="373"/>
-      <c r="F10" s="373"/>
-      <c r="G10" s="373"/>
-      <c r="H10" s="373"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="357"/>
+      <c r="C10" s="394"/>
+      <c r="D10" s="394"/>
+      <c r="E10" s="394"/>
+      <c r="F10" s="394"/>
+      <c r="G10" s="394"/>
+      <c r="H10" s="394"/>
+      <c r="I10" s="394"/>
+      <c r="J10" s="394"/>
+      <c r="K10" s="394"/>
+      <c r="L10" s="394"/>
+      <c r="M10" s="394"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="366" t="s">
         <v>617</v>
       </c>
-      <c r="B11" s="373"/>
-      <c r="C11" s="373"/>
-      <c r="D11" s="373"/>
-      <c r="E11" s="373"/>
-      <c r="F11" s="373"/>
-      <c r="G11" s="373"/>
-      <c r="H11" s="373"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="357"/>
+      <c r="C11" s="394"/>
+      <c r="D11" s="394"/>
+      <c r="E11" s="394"/>
+      <c r="F11" s="394"/>
+      <c r="G11" s="394"/>
+      <c r="H11" s="394"/>
+      <c r="I11" s="394"/>
+      <c r="J11" s="394"/>
+      <c r="K11" s="394"/>
+      <c r="L11" s="394"/>
+      <c r="M11" s="394"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="366" t="s">
         <v>618</v>
       </c>
-      <c r="B12" s="373"/>
-      <c r="C12" s="373"/>
-      <c r="D12" s="373"/>
-      <c r="E12" s="373"/>
-      <c r="F12" s="373"/>
-      <c r="G12" s="373"/>
-      <c r="H12" s="373"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="357"/>
+      <c r="C12" s="394"/>
+      <c r="D12" s="394"/>
+      <c r="E12" s="394"/>
+      <c r="F12" s="394"/>
+      <c r="G12" s="394"/>
+      <c r="H12" s="394"/>
+      <c r="I12" s="394"/>
+      <c r="J12" s="394"/>
+      <c r="K12" s="394"/>
+      <c r="L12" s="394"/>
+      <c r="M12" s="394"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="366" t="s">
         <v>619</v>
       </c>
-      <c r="B13" s="373"/>
-      <c r="C13" s="373"/>
-      <c r="D13" s="373"/>
-      <c r="E13" s="373"/>
-      <c r="F13" s="373"/>
-      <c r="G13" s="373"/>
-      <c r="H13" s="373"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="357"/>
+      <c r="C13" s="394"/>
+      <c r="D13" s="394"/>
+      <c r="E13" s="394"/>
+      <c r="F13" s="394"/>
+      <c r="G13" s="394"/>
+      <c r="H13" s="394"/>
+      <c r="I13" s="394"/>
+      <c r="J13" s="394"/>
+      <c r="K13" s="394"/>
+      <c r="L13" s="394"/>
+      <c r="M13" s="394"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="366" t="s">
         <v>620</v>
       </c>
-      <c r="B14" s="373"/>
-      <c r="C14" s="373"/>
-      <c r="D14" s="373"/>
-      <c r="E14" s="373"/>
-      <c r="F14" s="373"/>
-      <c r="G14" s="373"/>
-      <c r="H14" s="373"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="357"/>
+      <c r="C14" s="394"/>
+      <c r="D14" s="394"/>
+      <c r="E14" s="394"/>
+      <c r="F14" s="394"/>
+      <c r="G14" s="394"/>
+      <c r="H14" s="394"/>
+      <c r="I14" s="394"/>
+      <c r="J14" s="394"/>
+      <c r="K14" s="394"/>
+      <c r="L14" s="394"/>
+      <c r="M14" s="394"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="366" t="s">
         <v>621</v>
       </c>
-      <c r="B15" s="373"/>
-      <c r="C15" s="373"/>
-      <c r="D15" s="373"/>
-      <c r="E15" s="373"/>
-      <c r="F15" s="373"/>
-      <c r="G15" s="373"/>
-      <c r="H15" s="373"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="357"/>
+      <c r="C15" s="394"/>
+      <c r="D15" s="394"/>
+      <c r="E15" s="394"/>
+      <c r="F15" s="394"/>
+      <c r="G15" s="394"/>
+      <c r="H15" s="394"/>
+      <c r="I15" s="394"/>
+      <c r="J15" s="394"/>
+      <c r="K15" s="394"/>
+      <c r="L15" s="394"/>
+      <c r="M15" s="394"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="366" t="s">
         <v>622</v>
       </c>
-      <c r="B16" s="373"/>
-      <c r="C16" s="373"/>
-      <c r="D16" s="373"/>
-      <c r="E16" s="373"/>
-      <c r="F16" s="373"/>
-      <c r="G16" s="373"/>
-      <c r="H16" s="373"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="357"/>
+      <c r="C16" s="394"/>
+      <c r="D16" s="394"/>
+      <c r="E16" s="394"/>
+      <c r="F16" s="394"/>
+      <c r="G16" s="394"/>
+      <c r="H16" s="394"/>
+      <c r="I16" s="394"/>
+      <c r="J16" s="394"/>
+      <c r="K16" s="394"/>
+      <c r="L16" s="394"/>
+      <c r="M16" s="394"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="366" t="s">
         <v>623</v>
       </c>
-      <c r="B17" s="373"/>
-      <c r="C17" s="373"/>
-      <c r="D17" s="373"/>
-      <c r="E17" s="373"/>
-      <c r="F17" s="373"/>
-      <c r="G17" s="373"/>
-      <c r="H17" s="373"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="357"/>
+      <c r="C17" s="394"/>
+      <c r="D17" s="394"/>
+      <c r="E17" s="394"/>
+      <c r="F17" s="394"/>
+      <c r="G17" s="394"/>
+      <c r="H17" s="394"/>
+      <c r="I17" s="394"/>
+      <c r="J17" s="394"/>
+      <c r="K17" s="394"/>
+      <c r="L17" s="394"/>
+      <c r="M17" s="394"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="366" t="s">
         <v>624</v>
       </c>
-      <c r="B18" s="373"/>
-      <c r="C18" s="373"/>
-      <c r="D18" s="373"/>
-      <c r="E18" s="373"/>
-      <c r="F18" s="373"/>
-      <c r="G18" s="373"/>
-      <c r="H18" s="373"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="357"/>
+      <c r="C18" s="394"/>
+      <c r="D18" s="394"/>
+      <c r="E18" s="394"/>
+      <c r="F18" s="394"/>
+      <c r="G18" s="394"/>
+      <c r="H18" s="394"/>
+      <c r="I18" s="394"/>
+      <c r="J18" s="394"/>
+      <c r="K18" s="394"/>
+      <c r="L18" s="394"/>
+      <c r="M18" s="394"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="366" t="s">
         <v>625</v>
       </c>
-      <c r="B19" s="373"/>
-      <c r="C19" s="373"/>
-      <c r="D19" s="373"/>
-      <c r="E19" s="373"/>
-      <c r="F19" s="373"/>
-      <c r="G19" s="373"/>
-      <c r="H19" s="373"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="357"/>
+      <c r="C19" s="394"/>
+      <c r="D19" s="394"/>
+      <c r="E19" s="394"/>
+      <c r="F19" s="394"/>
+      <c r="G19" s="394"/>
+      <c r="H19" s="394"/>
+      <c r="I19" s="394"/>
+      <c r="J19" s="394"/>
+      <c r="K19" s="394"/>
+      <c r="L19" s="394"/>
+      <c r="M19" s="394"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="366" t="s">
         <v>626</v>
       </c>
-      <c r="B20" s="373"/>
-      <c r="C20" s="373"/>
-      <c r="D20" s="373"/>
-      <c r="E20" s="373"/>
-      <c r="F20" s="373"/>
-      <c r="G20" s="373"/>
-      <c r="H20" s="373"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="357"/>
+      <c r="C20" s="394"/>
+      <c r="D20" s="394"/>
+      <c r="E20" s="394"/>
+      <c r="F20" s="394"/>
+      <c r="G20" s="394"/>
+      <c r="H20" s="394"/>
+      <c r="I20" s="394"/>
+      <c r="J20" s="394"/>
+      <c r="K20" s="394"/>
+      <c r="L20" s="394"/>
+      <c r="M20" s="394"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="366" t="s">
         <v>627</v>
       </c>
-      <c r="B21" s="373"/>
-      <c r="C21" s="373"/>
-      <c r="D21" s="373"/>
-      <c r="E21" s="373"/>
-      <c r="F21" s="373"/>
-      <c r="G21" s="373"/>
-      <c r="H21" s="373"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="357"/>
+      <c r="C21" s="394"/>
+      <c r="D21" s="394"/>
+      <c r="E21" s="394"/>
+      <c r="F21" s="394"/>
+      <c r="G21" s="394"/>
+      <c r="H21" s="394"/>
+      <c r="I21" s="394"/>
+      <c r="J21" s="394"/>
+      <c r="K21" s="394"/>
+      <c r="L21" s="394"/>
+      <c r="M21" s="394"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="366" t="s">
         <v>628</v>
       </c>
-      <c r="B22" s="373"/>
-      <c r="C22" s="373"/>
-      <c r="D22" s="373"/>
-      <c r="E22" s="373"/>
-      <c r="F22" s="373"/>
-      <c r="G22" s="373"/>
-      <c r="H22" s="373"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="357"/>
+      <c r="C22" s="394"/>
+      <c r="D22" s="394"/>
+      <c r="E22" s="394"/>
+      <c r="F22" s="394"/>
+      <c r="G22" s="394"/>
+      <c r="H22" s="394"/>
+      <c r="I22" s="394"/>
+      <c r="J22" s="394"/>
+      <c r="K22" s="394"/>
+      <c r="L22" s="394"/>
+      <c r="M22" s="394"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="366" t="s">
         <v>629</v>
       </c>
-      <c r="B23" s="373"/>
-      <c r="C23" s="373"/>
-      <c r="D23" s="373"/>
-      <c r="E23" s="373"/>
-      <c r="F23" s="373"/>
-      <c r="G23" s="373"/>
-      <c r="H23" s="373"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="357"/>
+      <c r="C23" s="394"/>
+      <c r="D23" s="394"/>
+      <c r="E23" s="394"/>
+      <c r="F23" s="394"/>
+      <c r="G23" s="394"/>
+      <c r="H23" s="394"/>
+      <c r="I23" s="394"/>
+      <c r="J23" s="394"/>
+      <c r="K23" s="394"/>
+      <c r="L23" s="394"/>
+      <c r="M23" s="394"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="366" t="s">
         <v>630</v>
       </c>
-      <c r="B24" s="373"/>
-      <c r="C24" s="373"/>
-      <c r="D24" s="373"/>
-      <c r="E24" s="373"/>
-      <c r="F24" s="373"/>
-      <c r="G24" s="373"/>
-      <c r="H24" s="373"/>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="357"/>
+      <c r="C24" s="394"/>
+      <c r="D24" s="394"/>
+      <c r="E24" s="394"/>
+      <c r="F24" s="394"/>
+      <c r="G24" s="394"/>
+      <c r="H24" s="394"/>
+      <c r="I24" s="394"/>
+      <c r="J24" s="394"/>
+      <c r="K24" s="394"/>
+      <c r="L24" s="394"/>
+      <c r="M24" s="394"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="366" t="s">
         <v>631</v>
       </c>
-      <c r="B25" s="373"/>
-      <c r="C25" s="373"/>
-      <c r="D25" s="373"/>
-      <c r="E25" s="373"/>
-      <c r="F25" s="373"/>
-      <c r="G25" s="373"/>
-      <c r="H25" s="373"/>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="357"/>
+      <c r="C25" s="394"/>
+      <c r="D25" s="394"/>
+      <c r="E25" s="394"/>
+      <c r="F25" s="394"/>
+      <c r="G25" s="394"/>
+      <c r="H25" s="394"/>
+      <c r="I25" s="394"/>
+      <c r="J25" s="394"/>
+      <c r="K25" s="394"/>
+      <c r="L25" s="394"/>
+      <c r="M25" s="394"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="366" t="s">
         <v>632</v>
       </c>
-      <c r="B26" s="373"/>
-      <c r="C26" s="373"/>
-      <c r="D26" s="373"/>
-      <c r="E26" s="373"/>
-      <c r="F26" s="373"/>
-      <c r="G26" s="373"/>
-      <c r="H26" s="373"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="357"/>
+      <c r="C26" s="394"/>
+      <c r="D26" s="394"/>
+      <c r="E26" s="394"/>
+      <c r="F26" s="394"/>
+      <c r="G26" s="394"/>
+      <c r="H26" s="394"/>
+      <c r="I26" s="394"/>
+      <c r="J26" s="394"/>
+      <c r="K26" s="394"/>
+      <c r="L26" s="394"/>
+      <c r="M26" s="394"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="366" t="s">
         <v>633</v>
       </c>
-      <c r="B27" s="373"/>
-      <c r="C27" s="373"/>
-      <c r="D27" s="373"/>
-      <c r="E27" s="373"/>
-      <c r="F27" s="373"/>
-      <c r="G27" s="373"/>
-      <c r="H27" s="373"/>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="357"/>
+      <c r="C27" s="394"/>
+      <c r="D27" s="394"/>
+      <c r="E27" s="394"/>
+      <c r="F27" s="394"/>
+      <c r="G27" s="394"/>
+      <c r="H27" s="394"/>
+      <c r="I27" s="394"/>
+      <c r="J27" s="394"/>
+      <c r="K27" s="394"/>
+      <c r="L27" s="394"/>
+      <c r="M27" s="394"/>
+      <c r="Q27" s="231"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="366" t="s">
         <v>634</v>
       </c>
-      <c r="B28" s="373"/>
-      <c r="C28" s="373"/>
-      <c r="D28" s="373"/>
-      <c r="E28" s="373"/>
-      <c r="F28" s="373"/>
-      <c r="G28" s="373"/>
-      <c r="H28" s="373"/>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="357"/>
+      <c r="C28" s="394"/>
+      <c r="D28" s="394"/>
+      <c r="E28" s="394"/>
+      <c r="F28" s="394"/>
+      <c r="G28" s="394"/>
+      <c r="H28" s="394"/>
+      <c r="I28" s="394"/>
+      <c r="J28" s="394"/>
+      <c r="K28" s="394"/>
+      <c r="L28" s="394"/>
+      <c r="M28" s="394"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="366" t="s">
         <v>635</v>
       </c>
-      <c r="B29" s="373"/>
-      <c r="C29" s="373"/>
-      <c r="D29" s="373"/>
-      <c r="E29" s="373"/>
-      <c r="F29" s="373"/>
-      <c r="G29" s="373"/>
-      <c r="H29" s="373"/>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="357"/>
+      <c r="C29" s="394"/>
+      <c r="D29" s="394"/>
+      <c r="E29" s="394"/>
+      <c r="F29" s="394"/>
+      <c r="G29" s="394"/>
+      <c r="H29" s="394"/>
+      <c r="I29" s="394"/>
+      <c r="J29" s="394"/>
+      <c r="K29" s="394"/>
+      <c r="L29" s="394"/>
+      <c r="M29" s="394"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="366" t="s">
         <v>636</v>
       </c>
-      <c r="B30" s="373"/>
-      <c r="C30" s="373"/>
-      <c r="D30" s="373"/>
-      <c r="E30" s="373"/>
-      <c r="F30" s="373"/>
-      <c r="G30" s="373"/>
-      <c r="H30" s="373"/>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="357"/>
+      <c r="C30" s="394"/>
+      <c r="D30" s="394"/>
+      <c r="E30" s="394"/>
+      <c r="F30" s="394"/>
+      <c r="G30" s="394"/>
+      <c r="H30" s="394"/>
+      <c r="I30" s="394"/>
+      <c r="J30" s="394"/>
+      <c r="K30" s="394"/>
+      <c r="L30" s="394"/>
+      <c r="M30" s="394"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="366" t="s">
         <v>637</v>
       </c>
-      <c r="B31" s="373"/>
-      <c r="C31" s="373"/>
-      <c r="D31" s="373"/>
-      <c r="E31" s="373"/>
-      <c r="F31" s="373"/>
-      <c r="G31" s="373"/>
-      <c r="H31" s="373"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="357"/>
+      <c r="C31" s="394"/>
+      <c r="D31" s="394"/>
+      <c r="E31" s="394"/>
+      <c r="F31" s="394"/>
+      <c r="G31" s="394"/>
+      <c r="H31" s="394"/>
+      <c r="I31" s="394"/>
+      <c r="J31" s="394"/>
+      <c r="K31" s="394"/>
+      <c r="L31" s="394"/>
+      <c r="M31" s="394"/>
+      <c r="P31" s="231"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="366" t="s">
         <v>638</v>
       </c>
-      <c r="B32" s="373"/>
-      <c r="C32" s="373"/>
-      <c r="D32" s="373"/>
-      <c r="E32" s="373"/>
-      <c r="F32" s="373"/>
-      <c r="G32" s="373"/>
-      <c r="H32" s="373"/>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="357"/>
+      <c r="C32" s="394"/>
+      <c r="D32" s="394"/>
+      <c r="E32" s="394"/>
+      <c r="F32" s="394"/>
+      <c r="G32" s="394"/>
+      <c r="H32" s="394"/>
+      <c r="I32" s="394"/>
+      <c r="J32" s="394"/>
+      <c r="K32" s="394"/>
+      <c r="L32" s="394"/>
+      <c r="M32" s="394"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="366" t="s">
         <v>639</v>
       </c>
-      <c r="B33" s="373"/>
-      <c r="C33" s="373"/>
-      <c r="D33" s="373"/>
-      <c r="E33" s="373"/>
-      <c r="F33" s="373"/>
-      <c r="G33" s="373"/>
-      <c r="H33" s="373"/>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="357"/>
+      <c r="C33" s="394"/>
+      <c r="D33" s="394"/>
+      <c r="E33" s="394"/>
+      <c r="F33" s="394"/>
+      <c r="G33" s="394"/>
+      <c r="H33" s="394"/>
+      <c r="I33" s="394"/>
+      <c r="J33" s="394"/>
+      <c r="K33" s="394"/>
+      <c r="L33" s="394"/>
+      <c r="M33" s="394"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="366" t="s">
         <v>640</v>
       </c>
-      <c r="B34" s="373"/>
-      <c r="C34" s="373"/>
-      <c r="D34" s="373"/>
-      <c r="E34" s="373"/>
-      <c r="F34" s="373"/>
-      <c r="G34" s="373"/>
-      <c r="H34" s="373"/>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="357"/>
+      <c r="C34" s="394"/>
+      <c r="D34" s="394"/>
+      <c r="E34" s="394"/>
+      <c r="F34" s="394"/>
+      <c r="G34" s="394"/>
+      <c r="H34" s="394"/>
+      <c r="I34" s="394"/>
+      <c r="J34" s="394"/>
+      <c r="K34" s="394"/>
+      <c r="L34" s="394"/>
+      <c r="M34" s="394"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="366" t="s">
         <v>641</v>
       </c>
-      <c r="B35" s="373"/>
-      <c r="C35" s="373"/>
-      <c r="D35" s="373"/>
-      <c r="E35" s="373"/>
-      <c r="F35" s="373"/>
-      <c r="G35" s="373"/>
-      <c r="H35" s="373"/>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="357"/>
+      <c r="C35" s="394"/>
+      <c r="D35" s="394"/>
+      <c r="E35" s="394"/>
+      <c r="F35" s="394"/>
+      <c r="G35" s="394"/>
+      <c r="H35" s="394"/>
+      <c r="I35" s="394"/>
+      <c r="J35" s="394"/>
+      <c r="K35" s="394"/>
+      <c r="L35" s="394"/>
+      <c r="M35" s="394"/>
+    </row>
+    <row r="36" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="366" t="s">
         <v>642</v>
       </c>
-      <c r="B36" s="373"/>
-      <c r="C36" s="373"/>
-      <c r="D36" s="373"/>
-      <c r="E36" s="373"/>
-      <c r="F36" s="373"/>
-      <c r="G36" s="373"/>
-      <c r="H36" s="373"/>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="395"/>
+      <c r="C36" s="396" t="s">
+        <v>643</v>
+      </c>
+      <c r="D36" s="397"/>
+      <c r="E36" s="397"/>
+      <c r="F36" s="397"/>
+      <c r="G36" s="397"/>
+      <c r="H36" s="397"/>
+      <c r="I36" s="397"/>
+      <c r="J36" s="397"/>
+      <c r="K36" s="397"/>
+      <c r="L36" s="397"/>
+      <c r="M36" s="398"/>
+    </row>
+    <row r="37" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="366" t="s">
-        <v>643</v>
-      </c>
-      <c r="B37" s="373"/>
-      <c r="C37" s="373"/>
-      <c r="D37" s="373"/>
-      <c r="E37" s="373"/>
-      <c r="F37" s="373"/>
-      <c r="G37" s="373"/>
-      <c r="H37" s="373"/>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>644</v>
+      </c>
+      <c r="B37" s="399"/>
+      <c r="C37" s="400"/>
+      <c r="D37" s="401" t="s">
+        <v>645</v>
+      </c>
+      <c r="E37" s="401"/>
+      <c r="F37" s="401"/>
+      <c r="G37" s="402" t="s">
+        <v>646</v>
+      </c>
+      <c r="H37" s="402"/>
+      <c r="I37" s="402"/>
+      <c r="J37" s="402" t="s">
+        <v>647</v>
+      </c>
+      <c r="K37" s="402"/>
+      <c r="L37" s="402" t="s">
+        <v>648</v>
+      </c>
+      <c r="M37" s="402"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="366" t="s">
-        <v>644</v>
-      </c>
-      <c r="B38" s="373"/>
-      <c r="C38" s="373"/>
-      <c r="D38" s="373"/>
-      <c r="E38" s="373"/>
-      <c r="F38" s="373"/>
-      <c r="G38" s="373"/>
-      <c r="H38" s="373"/>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>649</v>
+      </c>
+      <c r="B38" s="403"/>
+      <c r="C38" s="404" t="s">
+        <v>650</v>
+      </c>
+      <c r="D38" s="405" t="s">
+        <v>651</v>
+      </c>
+      <c r="E38" s="405"/>
+      <c r="F38" s="405"/>
+      <c r="G38" s="406" t="s">
+        <v>651</v>
+      </c>
+      <c r="H38" s="406"/>
+      <c r="I38" s="406"/>
+      <c r="J38" s="406" t="s">
+        <v>651</v>
+      </c>
+      <c r="K38" s="406"/>
+      <c r="L38" s="406" t="s">
+        <v>651</v>
+      </c>
+      <c r="M38" s="406"/>
+    </row>
+    <row r="39" customFormat="false" ht="24.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="366" t="s">
-        <v>645</v>
-      </c>
-      <c r="B39" s="373"/>
-      <c r="C39" s="373"/>
-      <c r="D39" s="373"/>
-      <c r="E39" s="373"/>
-      <c r="F39" s="373"/>
-      <c r="G39" s="373"/>
-      <c r="H39" s="373"/>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>652</v>
+      </c>
+      <c r="B39" s="407"/>
+      <c r="C39" s="408"/>
+      <c r="D39" s="409" t="s">
+        <v>296</v>
+      </c>
+      <c r="E39" s="410" t="s">
+        <v>299</v>
+      </c>
+      <c r="F39" s="410" t="s">
+        <v>653</v>
+      </c>
+      <c r="G39" s="410" t="s">
+        <v>297</v>
+      </c>
+      <c r="H39" s="410" t="s">
+        <v>654</v>
+      </c>
+      <c r="I39" s="410" t="s">
+        <v>655</v>
+      </c>
+      <c r="J39" s="410" t="s">
+        <v>305</v>
+      </c>
+      <c r="K39" s="410" t="s">
+        <v>306</v>
+      </c>
+      <c r="L39" s="410" t="s">
+        <v>305</v>
+      </c>
+      <c r="M39" s="410" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="366" t="s">
-        <v>646</v>
-      </c>
-      <c r="B40" s="373"/>
-      <c r="C40" s="373"/>
-      <c r="D40" s="373"/>
-      <c r="E40" s="373"/>
-      <c r="F40" s="373"/>
-      <c r="G40" s="373"/>
-      <c r="H40" s="373"/>
-    </row>
-    <row r="41" customFormat="false" ht="6.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>656</v>
+      </c>
+      <c r="B40" s="411"/>
+      <c r="C40" s="412" t="s">
+        <v>657</v>
+      </c>
+      <c r="D40" s="413" t="str">
+        <f aca="false">A11</f>
+        <v>[:tulokset :kuukausierittely 0 :tuotto :aurinkosahko]</v>
+      </c>
+      <c r="E40" s="413" t="str">
+        <f aca="false">A12</f>
+        <v>[:tulokset :kuukausierittely 0 :tuotto :tuulisahko]</v>
+      </c>
+      <c r="F40" s="413" t="str">
+        <f aca="false">A13</f>
+        <v>[:tulokset :kuukausierittely 0 :tuotto :muusahko]</v>
+      </c>
+      <c r="G40" s="413" t="str">
+        <f aca="false">A14</f>
+        <v>[:tulokset :kuukausierittely 0 :tuotto :aurinkolampo]</v>
+      </c>
+      <c r="H40" s="413" t="str">
+        <f aca="false">A15</f>
+        <v>[:tulokset :kuukausierittely 0 :tuotto :lampopumppu]</v>
+      </c>
+      <c r="I40" s="413" t="str">
+        <f aca="false">A16</f>
+        <v>[:tulokset :kuukausierittely 0 :tuotto :muulampo]</v>
+      </c>
+      <c r="J40" s="413" t="str">
+        <f aca="false">A17</f>
+        <v>[:tulokset :kuukausierittely 0 :kulutus :sahko]</v>
+      </c>
+      <c r="K40" s="413" t="str">
+        <f aca="false">A18</f>
+        <v>[:tulokset :kuukausierittely 0 :kulutus :lampo]</v>
+      </c>
+      <c r="L40" s="413" t="str">
+        <f aca="false">A19</f>
+        <v>[:tulokset :kuukausierittely 0 :hyoty :sahko]</v>
+      </c>
+      <c r="M40" s="413" t="str">
+        <f aca="false">A20</f>
+        <v>[:tulokset :kuukausierittely 0 :hyoty :lampo]</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="366" t="s">
-        <v>647</v>
-      </c>
-      <c r="B41" s="373"/>
-      <c r="C41" s="373"/>
-      <c r="D41" s="373"/>
-      <c r="E41" s="373"/>
-      <c r="F41" s="373"/>
-      <c r="G41" s="373"/>
-      <c r="H41" s="373"/>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>658</v>
+      </c>
+      <c r="B41" s="411"/>
+      <c r="C41" s="412" t="s">
+        <v>659</v>
+      </c>
+      <c r="D41" s="413" t="str">
+        <f aca="false">A21</f>
+        <v>[:tulokset :kuukausierittely 1 :tuotto :aurinkosahko]</v>
+      </c>
+      <c r="E41" s="413" t="str">
+        <f aca="false">A22</f>
+        <v>[:tulokset :kuukausierittely 1 :tuotto :tuulisahko]</v>
+      </c>
+      <c r="F41" s="413" t="str">
+        <f aca="false">A23</f>
+        <v>[:tulokset :kuukausierittely 1 :tuotto :muusahko]</v>
+      </c>
+      <c r="G41" s="413" t="str">
+        <f aca="false">A24</f>
+        <v>[:tulokset :kuukausierittely 1 :tuotto :aurinkolampo]</v>
+      </c>
+      <c r="H41" s="413" t="str">
+        <f aca="false">A25</f>
+        <v>[:tulokset :kuukausierittely 1 :tuotto :lampopumppu]</v>
+      </c>
+      <c r="I41" s="413" t="str">
+        <f aca="false">A26</f>
+        <v>[:tulokset :kuukausierittely 1 :tuotto :muulampo]</v>
+      </c>
+      <c r="J41" s="413" t="str">
+        <f aca="false">A27</f>
+        <v>[:tulokset :kuukausierittely 1 :kulutus :sahko]</v>
+      </c>
+      <c r="K41" s="413" t="str">
+        <f aca="false">A28</f>
+        <v>[:tulokset :kuukausierittely 1 :kulutus :lampo]</v>
+      </c>
+      <c r="L41" s="413" t="str">
+        <f aca="false">A29</f>
+        <v>[:tulokset :kuukausierittely 1 :hyoty :sahko]</v>
+      </c>
+      <c r="M41" s="413" t="str">
+        <f aca="false">A30</f>
+        <v>[:tulokset :kuukausierittely 1 :hyoty :lampo]</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="366" t="s">
-        <v>648</v>
-      </c>
-      <c r="B42" s="373"/>
-      <c r="C42" s="373"/>
-      <c r="D42" s="373"/>
-      <c r="E42" s="373"/>
-      <c r="F42" s="373"/>
-      <c r="G42" s="373"/>
-      <c r="H42" s="373"/>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>660</v>
+      </c>
+      <c r="B42" s="411"/>
+      <c r="C42" s="412" t="s">
+        <v>661</v>
+      </c>
+      <c r="D42" s="413" t="str">
+        <f aca="false">A31</f>
+        <v>[:tulokset :kuukausierittely 2 :tuotto :aurinkosahko]</v>
+      </c>
+      <c r="E42" s="413" t="str">
+        <f aca="false">A32</f>
+        <v>[:tulokset :kuukausierittely 2 :tuotto :tuulisahko]</v>
+      </c>
+      <c r="F42" s="413" t="str">
+        <f aca="false">A33</f>
+        <v>[:tulokset :kuukausierittely 2 :tuotto :muusahko]</v>
+      </c>
+      <c r="G42" s="413" t="str">
+        <f aca="false">A34</f>
+        <v>[:tulokset :kuukausierittely 2 :tuotto :aurinkolampo]</v>
+      </c>
+      <c r="H42" s="413" t="str">
+        <f aca="false">A35</f>
+        <v>[:tulokset :kuukausierittely 2 :tuotto :lampopumppu]</v>
+      </c>
+      <c r="I42" s="413" t="str">
+        <f aca="false">A36</f>
+        <v>[:tulokset :kuukausierittely 2 :tuotto :muulampo]</v>
+      </c>
+      <c r="J42" s="413" t="str">
+        <f aca="false">A37</f>
+        <v>[:tulokset :kuukausierittely 2 :kulutus :sahko]</v>
+      </c>
+      <c r="K42" s="413" t="str">
+        <f aca="false">A38</f>
+        <v>[:tulokset :kuukausierittely 2 :kulutus :lampo]</v>
+      </c>
+      <c r="L42" s="413" t="str">
+        <f aca="false">A39</f>
+        <v>[:tulokset :kuukausierittely 2 :hyoty :sahko]</v>
+      </c>
+      <c r="M42" s="413" t="str">
+        <f aca="false">A40</f>
+        <v>[:tulokset :kuukausierittely 2 :hyoty :lampo]</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="366" t="s">
-        <v>649</v>
-      </c>
-      <c r="B43" s="373"/>
-      <c r="C43" s="373"/>
-      <c r="D43" s="373"/>
-      <c r="E43" s="373"/>
-      <c r="F43" s="373"/>
-      <c r="G43" s="373"/>
-      <c r="H43" s="373"/>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>662</v>
+      </c>
+      <c r="B43" s="411"/>
+      <c r="C43" s="412" t="s">
+        <v>663</v>
+      </c>
+      <c r="D43" s="413" t="str">
+        <f aca="false">A41</f>
+        <v>[:tulokset :kuukausierittely 3 :tuotto :aurinkosahko]</v>
+      </c>
+      <c r="E43" s="413" t="str">
+        <f aca="false">A42</f>
+        <v>[:tulokset :kuukausierittely 3 :tuotto :tuulisahko]</v>
+      </c>
+      <c r="F43" s="413" t="str">
+        <f aca="false">A43</f>
+        <v>[:tulokset :kuukausierittely 3 :tuotto :muusahko]</v>
+      </c>
+      <c r="G43" s="413" t="str">
+        <f aca="false">A44</f>
+        <v>[:tulokset :kuukausierittely 3 :tuotto :aurinkolampo]</v>
+      </c>
+      <c r="H43" s="413" t="str">
+        <f aca="false">A45</f>
+        <v>[:tulokset :kuukausierittely 3 :tuotto :lampopumppu]</v>
+      </c>
+      <c r="I43" s="413" t="str">
+        <f aca="false">A46</f>
+        <v>[:tulokset :kuukausierittely 3 :tuotto :muulampo]</v>
+      </c>
+      <c r="J43" s="413" t="str">
+        <f aca="false">A47</f>
+        <v>[:tulokset :kuukausierittely 3 :kulutus :sahko]</v>
+      </c>
+      <c r="K43" s="413" t="str">
+        <f aca="false">A48</f>
+        <v>[:tulokset :kuukausierittely 3 :kulutus :lampo]</v>
+      </c>
+      <c r="L43" s="413" t="str">
+        <f aca="false">A49</f>
+        <v>[:tulokset :kuukausierittely 3 :hyoty :sahko]</v>
+      </c>
+      <c r="M43" s="413" t="str">
+        <f aca="false">A50</f>
+        <v>[:tulokset :kuukausierittely 3 :hyoty :lampo]</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="366" t="s">
-        <v>650</v>
-      </c>
-      <c r="B44" s="373"/>
-      <c r="C44" s="373"/>
-      <c r="D44" s="373"/>
-      <c r="E44" s="373"/>
-      <c r="F44" s="373"/>
-      <c r="G44" s="373"/>
-      <c r="H44" s="373"/>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>664</v>
+      </c>
+      <c r="B44" s="411"/>
+      <c r="C44" s="412" t="s">
+        <v>665</v>
+      </c>
+      <c r="D44" s="413" t="str">
+        <f aca="false">A51</f>
+        <v>[:tulokset :kuukausierittely 4 :tuotto :aurinkosahko]</v>
+      </c>
+      <c r="E44" s="413" t="str">
+        <f aca="false">A52</f>
+        <v>[:tulokset :kuukausierittely 4 :tuotto :tuulisahko]</v>
+      </c>
+      <c r="F44" s="413" t="str">
+        <f aca="false">A53</f>
+        <v>[:tulokset :kuukausierittely 4 :tuotto :muusahko]</v>
+      </c>
+      <c r="G44" s="413" t="str">
+        <f aca="false">A54</f>
+        <v>[:tulokset :kuukausierittely 4 :tuotto :aurinkolampo]</v>
+      </c>
+      <c r="H44" s="413" t="str">
+        <f aca="false">A55</f>
+        <v>[:tulokset :kuukausierittely 4 :tuotto :lampopumppu]</v>
+      </c>
+      <c r="I44" s="413" t="str">
+        <f aca="false">A56</f>
+        <v>[:tulokset :kuukausierittely 4 :tuotto :muulampo]</v>
+      </c>
+      <c r="J44" s="413" t="str">
+        <f aca="false">A57</f>
+        <v>[:tulokset :kuukausierittely 4 :kulutus :sahko]</v>
+      </c>
+      <c r="K44" s="413" t="str">
+        <f aca="false">A58</f>
+        <v>[:tulokset :kuukausierittely 4 :kulutus :lampo]</v>
+      </c>
+      <c r="L44" s="413" t="str">
+        <f aca="false">A59</f>
+        <v>[:tulokset :kuukausierittely 4 :hyoty :sahko]</v>
+      </c>
+      <c r="M44" s="413" t="str">
+        <f aca="false">A60</f>
+        <v>[:tulokset :kuukausierittely 4 :hyoty :lampo]</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="366" t="s">
-        <v>651</v>
-      </c>
-      <c r="B45" s="373"/>
-      <c r="C45" s="373"/>
-      <c r="D45" s="373"/>
-      <c r="E45" s="373"/>
-      <c r="F45" s="373"/>
-      <c r="G45" s="373"/>
-      <c r="H45" s="373"/>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>666</v>
+      </c>
+      <c r="B45" s="411"/>
+      <c r="C45" s="412" t="s">
+        <v>667</v>
+      </c>
+      <c r="D45" s="413" t="str">
+        <f aca="false">A61</f>
+        <v>[:tulokset :kuukausierittely 5 :tuotto :aurinkosahko]</v>
+      </c>
+      <c r="E45" s="413" t="str">
+        <f aca="false">A62</f>
+        <v>[:tulokset :kuukausierittely 5 :tuotto :tuulisahko]</v>
+      </c>
+      <c r="F45" s="413" t="str">
+        <f aca="false">A63</f>
+        <v>[:tulokset :kuukausierittely 5 :tuotto :muusahko]</v>
+      </c>
+      <c r="G45" s="413" t="str">
+        <f aca="false">A64</f>
+        <v>[:tulokset :kuukausierittely 5 :tuotto :aurinkolampo]</v>
+      </c>
+      <c r="H45" s="413" t="str">
+        <f aca="false">A65</f>
+        <v>[:tulokset :kuukausierittely 5 :tuotto :lampopumppu]</v>
+      </c>
+      <c r="I45" s="413" t="str">
+        <f aca="false">A66</f>
+        <v>[:tulokset :kuukausierittely 5 :tuotto :muulampo]</v>
+      </c>
+      <c r="J45" s="413" t="str">
+        <f aca="false">A67</f>
+        <v>[:tulokset :kuukausierittely 5 :kulutus :sahko]</v>
+      </c>
+      <c r="K45" s="413" t="str">
+        <f aca="false">A68</f>
+        <v>[:tulokset :kuukausierittely 5 :kulutus :lampo]</v>
+      </c>
+      <c r="L45" s="413" t="str">
+        <f aca="false">A69</f>
+        <v>[:tulokset :kuukausierittely 5 :hyoty :sahko]</v>
+      </c>
+      <c r="M45" s="413" t="str">
+        <f aca="false">A70</f>
+        <v>[:tulokset :kuukausierittely 5 :hyoty :lampo]</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="366" t="s">
-        <v>652</v>
-      </c>
-      <c r="B46" s="373"/>
-      <c r="C46" s="373"/>
-      <c r="D46" s="373"/>
-      <c r="E46" s="373"/>
-      <c r="F46" s="373"/>
-      <c r="G46" s="373"/>
-      <c r="H46" s="373"/>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>668</v>
+      </c>
+      <c r="B46" s="411"/>
+      <c r="C46" s="412" t="s">
+        <v>669</v>
+      </c>
+      <c r="D46" s="413" t="str">
+        <f aca="false">A71</f>
+        <v>[:tulokset :kuukausierittely 6 :tuotto :aurinkosahko]</v>
+      </c>
+      <c r="E46" s="413" t="str">
+        <f aca="false">A72</f>
+        <v>[:tulokset :kuukausierittely 6 :tuotto :tuulisahko]</v>
+      </c>
+      <c r="F46" s="413" t="str">
+        <f aca="false">A73</f>
+        <v>[:tulokset :kuukausierittely 6 :tuotto :muusahko]</v>
+      </c>
+      <c r="G46" s="413" t="str">
+        <f aca="false">A74</f>
+        <v>[:tulokset :kuukausierittely 6 :tuotto :aurinkolampo]</v>
+      </c>
+      <c r="H46" s="413" t="str">
+        <f aca="false">A75</f>
+        <v>[:tulokset :kuukausierittely 6 :tuotto :lampopumppu]</v>
+      </c>
+      <c r="I46" s="413" t="str">
+        <f aca="false">A76</f>
+        <v>[:tulokset :kuukausierittely 6 :tuotto :muulampo]</v>
+      </c>
+      <c r="J46" s="413" t="str">
+        <f aca="false">A77</f>
+        <v>[:tulokset :kuukausierittely 6 :kulutus :sahko]</v>
+      </c>
+      <c r="K46" s="413" t="str">
+        <f aca="false">A78</f>
+        <v>[:tulokset :kuukausierittely 6 :kulutus :lampo]</v>
+      </c>
+      <c r="L46" s="413" t="str">
+        <f aca="false">A79</f>
+        <v>[:tulokset :kuukausierittely 6 :hyoty :sahko]</v>
+      </c>
+      <c r="M46" s="413" t="str">
+        <f aca="false">A80</f>
+        <v>[:tulokset :kuukausierittely 6 :hyoty :lampo]</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="366" t="s">
-        <v>653</v>
-      </c>
-      <c r="B47" s="373"/>
-      <c r="C47" s="373"/>
-      <c r="D47" s="373"/>
-      <c r="E47" s="373"/>
-      <c r="F47" s="373"/>
-      <c r="G47" s="373"/>
-      <c r="H47" s="373"/>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>670</v>
+      </c>
+      <c r="B47" s="411"/>
+      <c r="C47" s="412" t="s">
+        <v>671</v>
+      </c>
+      <c r="D47" s="413" t="str">
+        <f aca="false">A81</f>
+        <v>[:tulokset :kuukausierittely 7 :tuotto :aurinkosahko]</v>
+      </c>
+      <c r="E47" s="413" t="str">
+        <f aca="false">A82</f>
+        <v>[:tulokset :kuukausierittely 7 :tuotto :tuulisahko]</v>
+      </c>
+      <c r="F47" s="413" t="str">
+        <f aca="false">A83</f>
+        <v>[:tulokset :kuukausierittely 7 :tuotto :muusahko]</v>
+      </c>
+      <c r="G47" s="413" t="str">
+        <f aca="false">A84</f>
+        <v>[:tulokset :kuukausierittely 7 :tuotto :aurinkolampo]</v>
+      </c>
+      <c r="H47" s="413" t="str">
+        <f aca="false">A85</f>
+        <v>[:tulokset :kuukausierittely 7 :tuotto :lampopumppu]</v>
+      </c>
+      <c r="I47" s="413" t="str">
+        <f aca="false">A86</f>
+        <v>[:tulokset :kuukausierittely 7 :tuotto :muulampo]</v>
+      </c>
+      <c r="J47" s="413" t="str">
+        <f aca="false">A87</f>
+        <v>[:tulokset :kuukausierittely 7 :kulutus :sahko]</v>
+      </c>
+      <c r="K47" s="413" t="str">
+        <f aca="false">A88</f>
+        <v>[:tulokset :kuukausierittely 7 :kulutus :lampo]</v>
+      </c>
+      <c r="L47" s="413" t="str">
+        <f aca="false">A89</f>
+        <v>[:tulokset :kuukausierittely 7 :hyoty :sahko]</v>
+      </c>
+      <c r="M47" s="413" t="str">
+        <f aca="false">A90</f>
+        <v>[:tulokset :kuukausierittely 7 :hyoty :lampo]</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="366" t="s">
-        <v>654</v>
-      </c>
-      <c r="B48" s="373"/>
-      <c r="C48" s="373"/>
-      <c r="D48" s="373"/>
-      <c r="E48" s="373"/>
-      <c r="F48" s="373"/>
-      <c r="G48" s="373"/>
-      <c r="H48" s="373"/>
-    </row>
-    <row r="49" customFormat="false" ht="19.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>672</v>
+      </c>
+      <c r="B48" s="411"/>
+      <c r="C48" s="412" t="s">
+        <v>673</v>
+      </c>
+      <c r="D48" s="413" t="str">
+        <f aca="false">A91</f>
+        <v>[:tulokset :kuukausierittely 8 :tuotto :aurinkosahko]</v>
+      </c>
+      <c r="E48" s="413" t="str">
+        <f aca="false">A92</f>
+        <v>[:tulokset :kuukausierittely 8 :tuotto :tuulisahko]</v>
+      </c>
+      <c r="F48" s="413" t="str">
+        <f aca="false">A93</f>
+        <v>[:tulokset :kuukausierittely 8 :tuotto :muusahko]</v>
+      </c>
+      <c r="G48" s="413" t="str">
+        <f aca="false">A94</f>
+        <v>[:tulokset :kuukausierittely 8 :tuotto :aurinkolampo]</v>
+      </c>
+      <c r="H48" s="413" t="str">
+        <f aca="false">A95</f>
+        <v>[:tulokset :kuukausierittely 8 :tuotto :lampopumppu]</v>
+      </c>
+      <c r="I48" s="413" t="str">
+        <f aca="false">A96</f>
+        <v>[:tulokset :kuukausierittely 8 :tuotto :muulampo]</v>
+      </c>
+      <c r="J48" s="413" t="str">
+        <f aca="false">A97</f>
+        <v>[:tulokset :kuukausierittely 8 :kulutus :sahko]</v>
+      </c>
+      <c r="K48" s="413" t="str">
+        <f aca="false">A98</f>
+        <v>[:tulokset :kuukausierittely 8 :kulutus :lampo]</v>
+      </c>
+      <c r="L48" s="413" t="str">
+        <f aca="false">A99</f>
+        <v>[:tulokset :kuukausierittely 8 :hyoty :sahko]</v>
+      </c>
+      <c r="M48" s="413" t="str">
+        <f aca="false">A100</f>
+        <v>[:tulokset :kuukausierittely 8 :hyoty :lampo]</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="366" t="s">
-        <v>655</v>
-      </c>
-      <c r="B49" s="373"/>
-      <c r="C49" s="373"/>
-      <c r="D49" s="373"/>
-      <c r="E49" s="373"/>
-      <c r="F49" s="373"/>
-      <c r="G49" s="373"/>
-      <c r="H49" s="373"/>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>674</v>
+      </c>
+      <c r="B49" s="411"/>
+      <c r="C49" s="412" t="s">
+        <v>675</v>
+      </c>
+      <c r="D49" s="413" t="str">
+        <f aca="false">A101</f>
+        <v>[:tulokset :kuukausierittely 9 :tuotto :aurinkosahko]</v>
+      </c>
+      <c r="E49" s="413" t="str">
+        <f aca="false">A102</f>
+        <v>[:tulokset :kuukausierittely 9 :tuotto :tuulisahko]</v>
+      </c>
+      <c r="F49" s="413" t="str">
+        <f aca="false">A103</f>
+        <v>[:tulokset :kuukausierittely 9 :tuotto :muusahko]</v>
+      </c>
+      <c r="G49" s="413" t="str">
+        <f aca="false">A104</f>
+        <v>[:tulokset :kuukausierittely 9 :tuotto :aurinkolampo]</v>
+      </c>
+      <c r="H49" s="413" t="str">
+        <f aca="false">A105</f>
+        <v>[:tulokset :kuukausierittely 9 :tuotto :lampopumppu]</v>
+      </c>
+      <c r="I49" s="413" t="str">
+        <f aca="false">A106</f>
+        <v>[:tulokset :kuukausierittely 9 :tuotto :muulampo]</v>
+      </c>
+      <c r="J49" s="413" t="str">
+        <f aca="false">A107</f>
+        <v>[:tulokset :kuukausierittely 9 :kulutus :sahko]</v>
+      </c>
+      <c r="K49" s="413" t="str">
+        <f aca="false">A108</f>
+        <v>[:tulokset :kuukausierittely 9 :kulutus :lampo]</v>
+      </c>
+      <c r="L49" s="413" t="str">
+        <f aca="false">A109</f>
+        <v>[:tulokset :kuukausierittely 9 :hyoty :sahko]</v>
+      </c>
+      <c r="M49" s="413" t="str">
+        <f aca="false">A110</f>
+        <v>[:tulokset :kuukausierittely 9 :hyoty :lampo]</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="366" t="s">
-        <v>656</v>
-      </c>
-      <c r="B50" s="373"/>
-      <c r="C50" s="373"/>
-      <c r="D50" s="373"/>
-      <c r="E50" s="373"/>
-      <c r="F50" s="373"/>
-      <c r="G50" s="373"/>
-      <c r="H50" s="373"/>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>676</v>
+      </c>
+      <c r="B50" s="411"/>
+      <c r="C50" s="412" t="s">
+        <v>677</v>
+      </c>
+      <c r="D50" s="413" t="str">
+        <f aca="false">A111</f>
+        <v>[:tulokset :kuukausierittely 10 :tuotto :aurinkosahko]</v>
+      </c>
+      <c r="E50" s="413" t="str">
+        <f aca="false">A112</f>
+        <v>[:tulokset :kuukausierittely 10 :tuotto :tuulisahko]</v>
+      </c>
+      <c r="F50" s="413" t="str">
+        <f aca="false">A113</f>
+        <v>[:tulokset :kuukausierittely 10 :tuotto :muusahko]</v>
+      </c>
+      <c r="G50" s="413" t="str">
+        <f aca="false">A114</f>
+        <v>[:tulokset :kuukausierittely 10 :tuotto :aurinkolampo]</v>
+      </c>
+      <c r="H50" s="413" t="str">
+        <f aca="false">A115</f>
+        <v>[:tulokset :kuukausierittely 10 :tuotto :lampopumppu]</v>
+      </c>
+      <c r="I50" s="413" t="str">
+        <f aca="false">A116</f>
+        <v>[:tulokset :kuukausierittely 10 :tuotto :muulampo]</v>
+      </c>
+      <c r="J50" s="413" t="str">
+        <f aca="false">A117</f>
+        <v>[:tulokset :kuukausierittely 10 :kulutus :sahko]</v>
+      </c>
+      <c r="K50" s="413" t="str">
+        <f aca="false">A118</f>
+        <v>[:tulokset :kuukausierittely 10 :kulutus :lampo]</v>
+      </c>
+      <c r="L50" s="413" t="str">
+        <f aca="false">A119</f>
+        <v>[:tulokset :kuukausierittely 10 :hyoty :sahko]</v>
+      </c>
+      <c r="M50" s="413" t="str">
+        <f aca="false">A120</f>
+        <v>[:tulokset :kuukausierittely 10 :hyoty :lampo]</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="366" t="s">
-        <v>657</v>
-      </c>
-      <c r="B51" s="373"/>
-      <c r="C51" s="373"/>
-      <c r="D51" s="373"/>
-      <c r="E51" s="373"/>
-      <c r="F51" s="373"/>
-      <c r="G51" s="373"/>
-      <c r="H51" s="373"/>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>678</v>
+      </c>
+      <c r="B51" s="411"/>
+      <c r="C51" s="412" t="s">
+        <v>679</v>
+      </c>
+      <c r="D51" s="413" t="str">
+        <f aca="false">A121</f>
+        <v>[:tulokset :kuukausierittely 11 :tuotto :aurinkosahko]</v>
+      </c>
+      <c r="E51" s="413" t="str">
+        <f aca="false">A122</f>
+        <v>[:tulokset :kuukausierittely 11 :tuotto :tuulisahko]</v>
+      </c>
+      <c r="F51" s="413" t="str">
+        <f aca="false">A123</f>
+        <v>[:tulokset :kuukausierittely 11 :tuotto :muusahko]</v>
+      </c>
+      <c r="G51" s="413" t="str">
+        <f aca="false">A124</f>
+        <v>[:tulokset :kuukausierittely 11 :tuotto :aurinkolampo]</v>
+      </c>
+      <c r="H51" s="413" t="str">
+        <f aca="false">A125</f>
+        <v>[:tulokset :kuukausierittely 11 :tuotto :lampopumppu]</v>
+      </c>
+      <c r="I51" s="413" t="str">
+        <f aca="false">A126</f>
+        <v>[:tulokset :kuukausierittely 11 :tuotto :muulampo]</v>
+      </c>
+      <c r="J51" s="413" t="str">
+        <f aca="false">A127</f>
+        <v>[:tulokset :kuukausierittely 11 :kulutus :sahko]</v>
+      </c>
+      <c r="K51" s="413" t="str">
+        <f aca="false">A128</f>
+        <v>[:tulokset :kuukausierittely 11 :kulutus :lampo]</v>
+      </c>
+      <c r="L51" s="413" t="str">
+        <f aca="false">A129</f>
+        <v>[:tulokset :kuukausierittely 11 :hyoty :sahko]</v>
+      </c>
+      <c r="M51" s="413" t="str">
+        <f aca="false">A130</f>
+        <v>[:tulokset :kuukausierittely 11 :hyoty :lampo]</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="366" t="s">
-        <v>658</v>
-      </c>
-      <c r="B52" s="373"/>
-      <c r="C52" s="373"/>
-      <c r="D52" s="373"/>
-      <c r="E52" s="373"/>
-      <c r="F52" s="373"/>
-      <c r="G52" s="373"/>
-      <c r="H52" s="373"/>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>680</v>
+      </c>
+      <c r="B52" s="411"/>
+      <c r="C52" s="414" t="s">
+        <v>681</v>
+      </c>
+      <c r="D52" s="415" t="str">
+        <f aca="false">A131</f>
+        <v>[:tulokset :kuukausierittely-summat :tuotto :aurinkosahko]</v>
+      </c>
+      <c r="E52" s="415" t="str">
+        <f aca="false">A132</f>
+        <v>[:tulokset :kuukausierittely-summat :tuotto :tuulisahko]</v>
+      </c>
+      <c r="F52" s="415" t="str">
+        <f aca="false">A133</f>
+        <v>[:tulokset :kuukausierittely-summat :tuotto :muulampo]</v>
+      </c>
+      <c r="G52" s="415" t="str">
+        <f aca="false">A134</f>
+        <v>[:tulokset :kuukausierittely-summat :tuotto :aurinkolampo]</v>
+      </c>
+      <c r="H52" s="415" t="str">
+        <f aca="false">A135</f>
+        <v>[:tulokset :kuukausierittely-summat :tuotto :lampopumppu]</v>
+      </c>
+      <c r="I52" s="415" t="str">
+        <f aca="false">A136</f>
+        <v>[:tulokset :kuukausierittely-summat :tuotto :muulampo]</v>
+      </c>
+      <c r="J52" s="415" t="str">
+        <f aca="false">A137</f>
+        <v>[:tulokset :kuukausierittely-summat :kulutus :sahko]</v>
+      </c>
+      <c r="K52" s="415" t="str">
+        <f aca="false">A138</f>
+        <v>[:tulokset :kuukausierittely-summat :kulutus :lampo]</v>
+      </c>
+      <c r="L52" s="415" t="str">
+        <f aca="false">A139</f>
+        <v>[:tulokset :kuukausierittely-summat :hyoty :sahko]</v>
+      </c>
+      <c r="M52" s="415" t="str">
+        <f aca="false">A140</f>
+        <v>[:tulokset :kuukausierittely-summat :hyoty :lampo]</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="366" t="s">
-        <v>659</v>
-      </c>
-      <c r="B53" s="373"/>
-      <c r="C53" s="373"/>
-      <c r="D53" s="373"/>
-      <c r="E53" s="373"/>
-      <c r="F53" s="373"/>
-      <c r="G53" s="373"/>
-      <c r="H53" s="373"/>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>682</v>
+      </c>
+      <c r="B53" s="399"/>
+      <c r="C53" s="416" t="s">
+        <v>683</v>
+      </c>
+      <c r="D53" s="416"/>
+      <c r="E53" s="416"/>
+      <c r="F53" s="416"/>
+      <c r="G53" s="416"/>
+      <c r="H53" s="416"/>
+      <c r="I53" s="416"/>
+      <c r="J53" s="416"/>
+      <c r="K53" s="416"/>
+      <c r="L53" s="416"/>
+      <c r="M53" s="416"/>
+    </row>
+    <row r="54" customFormat="false" ht="7.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="366" t="s">
-        <v>660</v>
-      </c>
-      <c r="B54" s="373"/>
-      <c r="C54" s="373"/>
-      <c r="D54" s="373"/>
-      <c r="E54" s="373"/>
-      <c r="F54" s="373"/>
-      <c r="G54" s="373"/>
-      <c r="H54" s="373"/>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>684</v>
+      </c>
+      <c r="B54" s="399"/>
+      <c r="C54" s="417"/>
+      <c r="D54" s="417"/>
+      <c r="E54" s="417"/>
+      <c r="F54" s="417"/>
+      <c r="G54" s="417"/>
+      <c r="H54" s="417"/>
+      <c r="I54" s="417"/>
+      <c r="J54" s="417"/>
+      <c r="K54" s="417"/>
+      <c r="L54" s="417"/>
+      <c r="M54" s="400"/>
+    </row>
+    <row r="55" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="366" t="s">
-        <v>661</v>
-      </c>
-      <c r="B55" s="373"/>
-      <c r="C55" s="373"/>
-      <c r="D55" s="373"/>
-      <c r="E55" s="373"/>
-      <c r="F55" s="373"/>
-      <c r="G55" s="373"/>
-      <c r="H55" s="373"/>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>685</v>
+      </c>
+      <c r="B55" s="418"/>
+      <c r="C55" s="419" t="s">
+        <v>686</v>
+      </c>
+      <c r="D55" s="419"/>
+      <c r="E55" s="419"/>
+      <c r="F55" s="419"/>
+      <c r="G55" s="419"/>
+      <c r="H55" s="419"/>
+      <c r="I55" s="419"/>
+      <c r="J55" s="419"/>
+      <c r="K55" s="419"/>
+      <c r="L55" s="419"/>
+      <c r="M55" s="419"/>
+    </row>
+    <row r="56" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="366" t="s">
-        <v>662</v>
-      </c>
-      <c r="B56" s="373"/>
-      <c r="C56" s="373"/>
-      <c r="D56" s="373"/>
-      <c r="E56" s="373"/>
-      <c r="F56" s="373"/>
-      <c r="G56" s="373"/>
-      <c r="H56" s="373"/>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>687</v>
+      </c>
+      <c r="B56" s="420"/>
+      <c r="C56" s="421" t="s">
+        <v>688</v>
+      </c>
+      <c r="D56" s="421"/>
+      <c r="E56" s="421"/>
+      <c r="F56" s="421"/>
+      <c r="G56" s="421"/>
+      <c r="H56" s="421"/>
+      <c r="I56" s="421"/>
+      <c r="J56" s="422" t="str">
+        <f aca="false">A4</f>
+        <v>[:lahtotiedot :rakennusvaippa :lampokapasiteetti]</v>
+      </c>
+      <c r="K56" s="423"/>
+      <c r="L56" s="423"/>
+      <c r="M56" s="424"/>
+    </row>
+    <row r="57" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="366" t="s">
-        <v>663</v>
-      </c>
-      <c r="B57" s="373"/>
-      <c r="C57" s="373"/>
-      <c r="D57" s="373"/>
-      <c r="E57" s="373"/>
-      <c r="F57" s="373"/>
-      <c r="G57" s="373"/>
-      <c r="H57" s="373"/>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>689</v>
+      </c>
+      <c r="B57" s="420"/>
+      <c r="C57" s="421" t="s">
+        <v>690</v>
+      </c>
+      <c r="D57" s="421"/>
+      <c r="E57" s="421"/>
+      <c r="F57" s="421"/>
+      <c r="G57" s="421"/>
+      <c r="H57" s="421"/>
+      <c r="I57" s="421"/>
+      <c r="J57" s="422" t="str">
+        <f aca="false">A5</f>
+        <v>[:lahtotiedot :rakennusvaippa :ilmatilavuus]</v>
+      </c>
+      <c r="K57" s="423"/>
+      <c r="L57" s="423"/>
+      <c r="M57" s="424"/>
+    </row>
+    <row r="58" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="366" t="s">
-        <v>664</v>
-      </c>
-      <c r="B58" s="373"/>
-      <c r="C58" s="373"/>
-      <c r="D58" s="373"/>
-      <c r="E58" s="373"/>
-      <c r="F58" s="373"/>
-      <c r="G58" s="373"/>
-      <c r="H58" s="373"/>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>691</v>
+      </c>
+      <c r="B58" s="420"/>
+      <c r="C58" s="421" t="s">
+        <v>692</v>
+      </c>
+      <c r="D58" s="421"/>
+      <c r="E58" s="421"/>
+      <c r="F58" s="421"/>
+      <c r="G58" s="421"/>
+      <c r="H58" s="421"/>
+      <c r="I58" s="421"/>
+      <c r="J58" s="422" t="str">
+        <f aca="false">A6</f>
+        <v>[:lahtotiedot :ilmanvaihto :tuloilma-lampotila]</v>
+      </c>
+      <c r="K58" s="423"/>
+      <c r="L58" s="423"/>
+      <c r="M58" s="424"/>
+    </row>
+    <row r="59" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="366" t="s">
-        <v>665</v>
-      </c>
-      <c r="B59" s="373"/>
-      <c r="C59" s="373"/>
-      <c r="D59" s="373"/>
-      <c r="E59" s="373"/>
-      <c r="F59" s="373"/>
-      <c r="G59" s="373"/>
-      <c r="H59" s="373"/>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>693</v>
+      </c>
+      <c r="B59" s="420"/>
+      <c r="C59" s="421" t="s">
+        <v>694</v>
+      </c>
+      <c r="D59" s="421"/>
+      <c r="E59" s="421"/>
+      <c r="F59" s="421"/>
+      <c r="G59" s="421"/>
+      <c r="H59" s="421"/>
+      <c r="I59" s="421"/>
+      <c r="J59" s="422" t="str">
+        <f aca="false">A7</f>
+        <v>[:lahtotiedot :lammitys :tilat-ja-iv :lampopumppu-tuotto-osuus]</v>
+      </c>
+      <c r="K59" s="423"/>
+      <c r="L59" s="423"/>
+      <c r="M59" s="424"/>
+    </row>
+    <row r="60" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="366" t="s">
-        <v>666</v>
-      </c>
-      <c r="B60" s="373"/>
-      <c r="C60" s="373"/>
-      <c r="D60" s="373"/>
-      <c r="E60" s="373"/>
-      <c r="F60" s="373"/>
-      <c r="G60" s="373"/>
-      <c r="H60" s="373"/>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>695</v>
+      </c>
+      <c r="B60" s="420"/>
+      <c r="C60" s="421" t="s">
+        <v>696</v>
+      </c>
+      <c r="D60" s="421"/>
+      <c r="E60" s="421"/>
+      <c r="F60" s="421"/>
+      <c r="G60" s="421"/>
+      <c r="H60" s="421"/>
+      <c r="I60" s="421"/>
+      <c r="J60" s="422" t="str">
+        <f aca="false">A8</f>
+        <v>[:lahtotiedot :lammitys :lammin-kayttovesi :lampopumppu-tuotto-osuus]</v>
+      </c>
+      <c r="K60" s="423"/>
+      <c r="L60" s="423"/>
+      <c r="M60" s="424"/>
+    </row>
+    <row r="61" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="366" t="s">
-        <v>667</v>
-      </c>
-      <c r="B61" s="373"/>
-      <c r="C61" s="373"/>
-      <c r="D61" s="373"/>
-      <c r="E61" s="373"/>
-      <c r="F61" s="373"/>
-      <c r="G61" s="373"/>
-      <c r="H61" s="373"/>
+        <v>697</v>
+      </c>
+      <c r="B61" s="403"/>
+      <c r="C61" s="425" t="s">
+        <v>698</v>
+      </c>
+      <c r="D61" s="425"/>
+      <c r="E61" s="425"/>
+      <c r="F61" s="425"/>
+      <c r="G61" s="425"/>
+      <c r="H61" s="425"/>
+      <c r="I61" s="425"/>
+      <c r="J61" s="426" t="str">
+        <f aca="false">A9</f>
+        <v>[:lahtotiedot :lammitys :tilat-ja-iv :lampohavio-lammittamaton-tila]</v>
+      </c>
+      <c r="K61" s="427"/>
+      <c r="L61" s="427"/>
+      <c r="M61" s="428"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="366" t="s">
-        <v>668</v>
-      </c>
-      <c r="B62" s="393" t="str">
+        <v>699</v>
+      </c>
+      <c r="B62" s="429" t="str">
         <f aca="false">"Certifikatbeteckning: "&amp;A1&amp;", 8/8"</f>
         <v>Certifikatbeteckning: [:id], 8/8</v>
       </c>
-      <c r="C62" s="393"/>
-      <c r="D62" s="393"/>
-      <c r="E62" s="393"/>
-      <c r="F62" s="393"/>
-      <c r="G62" s="393"/>
-      <c r="H62" s="393"/>
+      <c r="C62" s="429"/>
+      <c r="D62" s="429"/>
+      <c r="E62" s="429"/>
+      <c r="F62" s="429"/>
+      <c r="G62" s="429"/>
+      <c r="H62" s="429"/>
+      <c r="I62" s="429"/>
+      <c r="J62" s="429"/>
+      <c r="K62" s="429"/>
+      <c r="L62" s="429"/>
+      <c r="M62" s="429"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="366" t="s">
-        <v>669</v>
-      </c>
-      <c r="B63" s="393"/>
-      <c r="C63" s="393"/>
-      <c r="D63" s="393"/>
-      <c r="E63" s="393"/>
-      <c r="F63" s="393"/>
-      <c r="G63" s="393"/>
-      <c r="H63" s="393"/>
+        <v>700</v>
+      </c>
+      <c r="B63" s="429"/>
+      <c r="C63" s="429"/>
+      <c r="D63" s="429"/>
+      <c r="E63" s="429"/>
+      <c r="F63" s="429"/>
+      <c r="G63" s="429"/>
+      <c r="H63" s="429"/>
+      <c r="I63" s="429"/>
+      <c r="J63" s="429"/>
+      <c r="K63" s="429"/>
+      <c r="L63" s="429"/>
+      <c r="M63" s="429"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="366" t="s">
-        <v>670</v>
+        <v>701</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="366" t="s">
-        <v>671</v>
+        <v>702</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="366" t="s">
-        <v>672</v>
+        <v>703</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="366" t="s">
-        <v>673</v>
+        <v>704</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="366" t="s">
-        <v>674</v>
+        <v>705</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="366" t="s">
-        <v>675</v>
+        <v>706</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="366" t="s">
-        <v>676</v>
+        <v>707</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="366" t="s">
-        <v>677</v>
+        <v>708</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="366" t="s">
-        <v>678</v>
+        <v>709</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="366" t="s">
-        <v>679</v>
+        <v>710</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="366" t="s">
-        <v>680</v>
+        <v>711</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="366" t="s">
-        <v>681</v>
+        <v>712</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="366" t="s">
-        <v>682</v>
+        <v>713</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="366" t="s">
-        <v>683</v>
+        <v>714</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="366" t="s">
-        <v>684</v>
+        <v>715</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="366" t="s">
-        <v>685</v>
+        <v>716</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="366" t="s">
-        <v>686</v>
+        <v>717</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="366" t="s">
-        <v>687</v>
+        <v>718</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="366" t="s">
-        <v>688</v>
+        <v>719</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="366" t="s">
-        <v>689</v>
+        <v>720</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="366" t="s">
-        <v>690</v>
+        <v>721</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="366" t="s">
-        <v>691</v>
+        <v>722</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="366" t="s">
-        <v>692</v>
+        <v>723</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="366" t="s">
-        <v>693</v>
+        <v>724</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="366" t="s">
-        <v>694</v>
+        <v>725</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="366" t="s">
-        <v>695</v>
+        <v>726</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="366" t="s">
-        <v>696</v>
+        <v>727</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="366" t="s">
-        <v>697</v>
+        <v>728</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="366" t="s">
-        <v>698</v>
+        <v>729</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="366" t="s">
-        <v>699</v>
+        <v>730</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="366" t="s">
-        <v>700</v>
+        <v>731</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="366" t="s">
-        <v>701</v>
+        <v>732</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="366" t="s">
-        <v>702</v>
+        <v>733</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="366" t="s">
-        <v>703</v>
+        <v>734</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="366" t="s">
-        <v>704</v>
+        <v>735</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="366" t="s">
-        <v>705</v>
+        <v>736</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="366" t="s">
-        <v>706</v>
+        <v>737</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="366" t="s">
-        <v>707</v>
+        <v>738</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="366" t="s">
-        <v>708</v>
+        <v>739</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="366" t="s">
-        <v>709</v>
+        <v>740</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="366" t="s">
-        <v>710</v>
+        <v>741</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="366" t="s">
-        <v>711</v>
+        <v>742</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="366" t="s">
-        <v>712</v>
+        <v>743</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="366" t="s">
-        <v>713</v>
+        <v>744</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="366" t="s">
-        <v>714</v>
+        <v>745</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="366" t="s">
-        <v>715</v>
+        <v>746</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="366" t="s">
-        <v>716</v>
+        <v>747</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="366" t="s">
-        <v>717</v>
+        <v>748</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="366" t="s">
-        <v>718</v>
+        <v>749</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="366" t="s">
-        <v>719</v>
+        <v>750</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="366" t="s">
-        <v>720</v>
+        <v>751</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="366" t="s">
-        <v>721</v>
+        <v>752</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="366" t="s">
-        <v>722</v>
+        <v>753</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="366" t="s">
-        <v>723</v>
+        <v>754</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="366" t="s">
-        <v>724</v>
+        <v>755</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="366" t="s">
-        <v>725</v>
+        <v>756</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="366" t="s">
-        <v>726</v>
+        <v>757</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="366" t="s">
-        <v>727</v>
+        <v>758</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="366" t="s">
-        <v>728</v>
+        <v>759</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="366" t="s">
-        <v>729</v>
+        <v>760</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="366" t="s">
-        <v>730</v>
+        <v>761</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="366" t="s">
-        <v>731</v>
+        <v>762</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="366" t="s">
-        <v>732</v>
+        <v>763</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="366" t="s">
-        <v>733</v>
+        <v>764</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="366" t="s">
-        <v>734</v>
+        <v>765</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="366" t="s">
-        <v>735</v>
+        <v>766</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="366" t="s">
-        <v>736</v>
+        <v>767</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="366" t="s">
-        <v>737</v>
+        <v>768</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="366" t="s">
-        <v>738</v>
+        <v>769</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="366" t="s">
-        <v>739</v>
+        <v>770</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="366" t="s">
-        <v>740</v>
+        <v>771</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="366" t="s">
-        <v>741</v>
+        <v>772</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="366" t="s">
-        <v>742</v>
+        <v>770</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="366" t="s">
-        <v>743</v>
+        <v>773</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="366" t="s">
-        <v>744</v>
+        <v>774</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="366" t="s">
-        <v>745</v>
+        <v>775</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="366" t="s">
-        <v>746</v>
+        <v>776</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B3:H61"/>
-    <mergeCell ref="B62:H63"/>
+  <mergeCells count="19">
+    <mergeCell ref="C2:M2"/>
+    <mergeCell ref="C3:M35"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="G37:I37"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="L37:M37"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="G38:I38"/>
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="L38:M38"/>
+    <mergeCell ref="C53:M53"/>
+    <mergeCell ref="C55:M55"/>
+    <mergeCell ref="C56:I56"/>
+    <mergeCell ref="C57:I57"/>
+    <mergeCell ref="C58:I58"/>
+    <mergeCell ref="C59:I59"/>
+    <mergeCell ref="C60:I60"/>
+    <mergeCell ref="C61:I61"/>
+    <mergeCell ref="B62:M63"/>
   </mergeCells>
-  <conditionalFormatting sqref="I2:AMJ2 A3:AMJ1048576">
+  <conditionalFormatting sqref="B62:AMJ1048576 B2:C2 N2:AMJ61 B55:M61 D40:M51 B38:B39 B36 A3:A1048576">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="317">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2">
-    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="308">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
-  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.709722222222222" right="0.709722222222222" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>

</xml_diff>

<commit_message>
AE-945 fix typos in sv templates
</commit_message>
<xml_diff>
--- a/etp-backend/src/main/resources/energiatodistus-2018-sv.xlsx
+++ b/etp-backend/src/main/resources/energiatodistus-2018-sv.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="1) etusivu" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,23 +19,23 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'1) etusivu'!$B$1:$R$51</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$58</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$59</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area" vbProcedure="false">'3) E-luvun laskennan lähtöt.'!$B$2:$G$67</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$2:$G$77</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$1:$G$78</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area" vbProcedure="false">'5) toteutunut kulutus'!$B$2:$K$55</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm.Print_Area" vbProcedure="false">'6) huomiot 1'!$B$2:$F$53</definedName>
-    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$60</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$61</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area" vbProcedure="false">'8) lisämerkintöjä'!$B$1:$M$63</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'1) etusivu'!$B$1:$R$50</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'2) E-luokka'!$B$2:$K$59</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$59</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$58</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'3) E-luvun laskennan lähtöt.'!$B$2:$G$66</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$2:$G$76</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$1:$G$78</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$2:$G$77</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'5) toteutunut kulutus'!$B$2:$L$54</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'6) huomiot 1'!$B$2:$G$52</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'7) huomiot 2'!$B$2:$G$59</definedName>
-    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$61</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$60</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -73,7 +73,7 @@
     <t xml:space="preserve">[:perustiedot :rakennustunnus]</t>
   </si>
   <si>
-    <t xml:space="preserve">Byggnadens namn och address:</t>
+    <t xml:space="preserve">Byggnadens namn och adress:</t>
   </si>
   <si>
     <t xml:space="preserve">[:perustiedot :valmistumisvuosi]</t>
@@ -322,6 +322,59 @@
     <t xml:space="preserve">-</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF009EE0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">kWh</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color rgb="FF009EE0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">E</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF009EE0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/(m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF009EE0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF009EE0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">år)</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">[:tulokset :kaytettavat-energiamuodot :sahko]</t>
   </si>
   <si>
@@ -1145,9 +1198,6 @@
     <t xml:space="preserve">st.</t>
   </si>
   <si>
-    <t xml:space="preserve">kWh</t>
-  </si>
-  <si>
     <t xml:space="preserve">[:lahtotiedot :ikkunat :luode :ala]</t>
   </si>
   <si>
@@ -1387,7 +1437,26 @@
     <t xml:space="preserve">BERÄKNING AV E-TAL, RESULTAT</t>
   </si>
   <si>
-    <t xml:space="preserve">Uppvärmd nettoarea, m 2</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF009EE0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Uppvärmd nettoarea, m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF009EE0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">2</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">[:tulokset :kaytettavat-energiamuodot :kaukolampo-kertoimella]</t>
@@ -3404,7 +3473,7 @@
     <numFmt numFmtId="173" formatCode="0%"/>
     <numFmt numFmtId="174" formatCode="0"/>
   </numFmts>
-  <fonts count="50">
+  <fonts count="52">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -3538,6 +3607,13 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="10"/>
+      <color rgb="FF009EE0"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -3675,6 +3751,13 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <color rgb="FF009EE0"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -4609,11 +4692,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4621,35 +4704,35 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="23" fillId="4" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="24" fillId="4" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="23" fillId="5" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="24" fillId="5" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="23" fillId="6" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="24" fillId="6" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="23" fillId="7" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="24" fillId="7" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="23" fillId="8" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="24" fillId="8" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="23" fillId="9" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="24" fillId="9" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4657,15 +4740,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="23" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="24" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4673,11 +4756,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4721,19 +4804,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4821,7 +4904,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="3" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="29" fillId="3" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4857,7 +4940,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -4905,7 +4988,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -4921,7 +5004,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -4937,11 +5020,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -4965,11 +5048,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -4985,7 +5068,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -4993,11 +5076,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -5025,7 +5108,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -5041,7 +5124,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -5065,7 +5148,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5149,7 +5232,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -5173,7 +5256,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="23" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="24" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -5217,15 +5300,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="41" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="169" fontId="43" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="40" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="42" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -5241,7 +5324,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5281,7 +5364,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="28" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5325,7 +5408,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="23" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5401,7 +5484,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="42" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="44" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5425,7 +5508,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="34" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="35" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -5473,11 +5556,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="43" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="45" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="43" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="45" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5493,11 +5576,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5513,7 +5596,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="44" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="46" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5537,7 +5620,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5621,7 +5704,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5641,7 +5724,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="45" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="47" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -5653,7 +5736,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="46" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="48" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5669,7 +5752,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="47" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="49" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -5685,7 +5768,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -5701,7 +5784,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="49" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="51" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -8085,9 +8168,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>229680</xdr:colOff>
+      <xdr:colOff>229320</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>244080</xdr:rowOff>
+      <xdr:rowOff>243720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8101,7 +8184,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="4656960"/>
-          <a:ext cx="739800" cy="196560"/>
+          <a:ext cx="739440" cy="196200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8122,9 +8205,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>129600</xdr:colOff>
+      <xdr:colOff>129240</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>244080</xdr:rowOff>
+      <xdr:rowOff>243720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8138,7 +8221,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="4971240"/>
-          <a:ext cx="1083240" cy="196560"/>
+          <a:ext cx="1082880" cy="196200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8159,9 +8242,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2880</xdr:colOff>
+      <xdr:colOff>2520</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>244080</xdr:rowOff>
+      <xdr:rowOff>243720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8175,7 +8258,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="5285520"/>
-          <a:ext cx="1389960" cy="196560"/>
+          <a:ext cx="1389600" cy="196200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8196,9 +8279,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>326880</xdr:colOff>
+      <xdr:colOff>326520</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>244080</xdr:rowOff>
+      <xdr:rowOff>243720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8212,7 +8295,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="5599800"/>
-          <a:ext cx="1713960" cy="196560"/>
+          <a:ext cx="1713600" cy="196200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8233,9 +8316,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>200160</xdr:colOff>
+      <xdr:colOff>199800</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>257040</xdr:rowOff>
+      <xdr:rowOff>256680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8249,7 +8332,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="5909760"/>
-          <a:ext cx="2021040" cy="209520"/>
+          <a:ext cx="2020680" cy="209160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8270,9 +8353,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>143280</xdr:colOff>
+      <xdr:colOff>142920</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>244080</xdr:rowOff>
+      <xdr:rowOff>243720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8286,7 +8369,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="6219720"/>
-          <a:ext cx="2357280" cy="196560"/>
+          <a:ext cx="2356920" cy="196200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8307,9 +8390,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>83520</xdr:colOff>
+      <xdr:colOff>83160</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>245160</xdr:rowOff>
+      <xdr:rowOff>244800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -8319,7 +8402,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="6531480"/>
-          <a:ext cx="2670120" cy="195480"/>
+          <a:ext cx="2669760" cy="195120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8688,9 +8771,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>282960</xdr:colOff>
+      <xdr:colOff>282600</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>84240</xdr:rowOff>
+      <xdr:rowOff>83880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -8700,7 +8783,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1978200" y="78480"/>
-          <a:ext cx="6969240" cy="10490760"/>
+          <a:ext cx="6968880" cy="10490400"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -8830,7 +8913,7 @@
   <dimension ref="A1:AMJ52"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L51" activeCellId="0" sqref="L51"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10478,8 +10561,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ65"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10854,7 +10937,7 @@
       <c r="Z11" s="0"/>
       <c r="AA11" s="0"/>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="99" t="s">
         <v>60</v>
       </c>
@@ -10872,7 +10955,7 @@
         <v>63</v>
       </c>
       <c r="I12" s="123" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J12" s="123"/>
       <c r="L12" s="0"/>
@@ -10894,7 +10977,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="99" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B13" s="107"/>
       <c r="C13" s="6"/>
@@ -10924,11 +11007,11 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="99" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B14" s="107"/>
       <c r="C14" s="129" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D14" s="129"/>
       <c r="E14" s="6"/>
@@ -10968,11 +11051,11 @@
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="99" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B15" s="107"/>
       <c r="C15" s="129" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D15" s="129"/>
       <c r="E15" s="6"/>
@@ -11012,11 +11095,11 @@
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="99" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B16" s="107"/>
       <c r="C16" s="129" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D16" s="129"/>
       <c r="E16" s="6"/>
@@ -11056,11 +11139,11 @@
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="99" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B17" s="107"/>
       <c r="C17" s="129" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D17" s="129"/>
       <c r="E17" s="6"/>
@@ -11100,11 +11183,11 @@
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="99" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B18" s="107"/>
       <c r="C18" s="129" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D18" s="129"/>
       <c r="E18" s="6"/>
@@ -11144,7 +11227,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="99" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B19" s="107"/>
       <c r="C19" s="129"/>
@@ -11174,11 +11257,11 @@
     </row>
     <row r="20" customFormat="false" ht="18.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="99" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B20" s="134"/>
       <c r="C20" s="135" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D20" s="135"/>
       <c r="E20" s="135"/>
@@ -11209,11 +11292,11 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="99" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B21" s="103"/>
       <c r="C21" s="104" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D21" s="104"/>
       <c r="E21" s="105"/>
@@ -11241,7 +11324,7 @@
     </row>
     <row r="22" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="99" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B22" s="107"/>
       <c r="C22" s="6"/>
@@ -11271,11 +11354,11 @@
     </row>
     <row r="23" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="99" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B23" s="107"/>
       <c r="C23" s="18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D23" s="18"/>
       <c r="E23" s="6"/>
@@ -11307,7 +11390,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="99" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B24" s="107"/>
       <c r="C24" s="18"/>
@@ -11337,11 +11420,11 @@
     </row>
     <row r="25" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="99" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B25" s="107"/>
       <c r="C25" s="18" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D25" s="18"/>
       <c r="E25" s="6"/>
@@ -11378,7 +11461,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="99" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B26" s="107"/>
       <c r="C26" s="18"/>
@@ -11417,7 +11500,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="99" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B27" s="107"/>
       <c r="C27" s="18"/>
@@ -11450,7 +11533,7 @@
     </row>
     <row r="28" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="99" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B28" s="107"/>
       <c r="C28" s="18"/>
@@ -11480,11 +11563,11 @@
     </row>
     <row r="29" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="99" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B29" s="107"/>
       <c r="C29" s="18" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D29" s="18"/>
       <c r="E29" s="6"/>
@@ -11515,7 +11598,7 @@
     </row>
     <row r="30" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="99" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B30" s="107"/>
       <c r="C30" s="140"/>
@@ -11545,11 +11628,11 @@
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="99" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B31" s="107"/>
       <c r="C31" s="153" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D31" s="153"/>
       <c r="E31" s="153"/>
@@ -11577,7 +11660,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="99" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B32" s="107"/>
       <c r="C32" s="153"/>
@@ -11607,7 +11690,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="99" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B33" s="107"/>
       <c r="C33" s="153"/>
@@ -11637,7 +11720,7 @@
     </row>
     <row r="34" customFormat="false" ht="17.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="99" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B34" s="107"/>
       <c r="C34" s="153"/>
@@ -11667,7 +11750,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="99" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B35" s="154"/>
       <c r="C35" s="155"/>
@@ -11701,7 +11784,7 @@
       </c>
       <c r="B36" s="157"/>
       <c r="C36" s="158" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D36" s="158"/>
       <c r="E36" s="158"/>
@@ -11729,11 +11812,11 @@
     </row>
     <row r="37" customFormat="false" ht="21.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="99" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B37" s="103"/>
       <c r="C37" s="104" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D37" s="104"/>
       <c r="E37" s="105"/>
@@ -11761,7 +11844,7 @@
     </row>
     <row r="38" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="99" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B38" s="160"/>
       <c r="C38" s="161" t="str">
@@ -11794,7 +11877,7 @@
     </row>
     <row r="39" s="4" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="99" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B39" s="107"/>
       <c r="C39" s="161"/>
@@ -11825,7 +11908,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="99" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B40" s="107"/>
       <c r="C40" s="161"/>
@@ -11855,7 +11938,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="99" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B41" s="107"/>
       <c r="C41" s="161"/>
@@ -11885,7 +11968,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="99" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B42" s="107"/>
       <c r="C42" s="161"/>
@@ -11915,7 +11998,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="162" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B43" s="107"/>
       <c r="C43" s="161"/>
@@ -11945,7 +12028,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="99" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B44" s="107"/>
       <c r="C44" s="161"/>
@@ -11975,7 +12058,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="99" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B45" s="107"/>
       <c r="C45" s="161"/>
@@ -12005,7 +12088,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="99" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B46" s="107"/>
       <c r="C46" s="161"/>
@@ -12035,7 +12118,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="99" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B47" s="107"/>
       <c r="C47" s="161"/>
@@ -12065,7 +12148,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="99" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B48" s="107"/>
       <c r="C48" s="161"/>
@@ -12311,7 +12394,7 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B57" s="163" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C57" s="163"/>
       <c r="D57" s="163"/>
@@ -12676,8 +12759,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ92"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C53" activeCellId="0" sqref="C53"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G45" activeCellId="0" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12700,7 +12783,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="169" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C2" s="169"/>
       <c r="D2" s="169"/>
@@ -12752,7 +12835,7 @@
       </c>
       <c r="B3" s="170"/>
       <c r="C3" s="171" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D3" s="172"/>
       <c r="E3" s="172"/>
@@ -12765,7 +12848,7 @@
       </c>
       <c r="B4" s="173"/>
       <c r="C4" s="174" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D4" s="175" t="str">
         <f aca="false">A3</f>
@@ -12782,11 +12865,11 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="162" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B5" s="173"/>
       <c r="C5" s="174" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D5" s="0" t="str">
         <f aca="false">A4</f>
@@ -12800,16 +12883,16 @@
         <v>[:lahtotiedot :lammitetty-nettoala]</v>
       </c>
       <c r="G5" s="177" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="162" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B6" s="178"/>
       <c r="C6" s="179" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D6" s="180"/>
       <c r="E6" s="181"/>
@@ -12818,67 +12901,67 @@
     </row>
     <row r="7" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="162" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B7" s="173"/>
       <c r="C7" s="174" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D7" s="183" t="str">
         <f aca="false">A6</f>
         <v>[:lahtotiedot :rakennusvaippa :ilmanvuotoluku]</v>
       </c>
       <c r="E7" s="184" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F7" s="185"/>
       <c r="G7" s="186"/>
     </row>
     <row r="8" customFormat="false" ht="20.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="162" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B8" s="173"/>
       <c r="C8" s="187"/>
       <c r="D8" s="188" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E8" s="188" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F8" s="188" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G8" s="189" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="162" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B9" s="173"/>
       <c r="C9" s="187"/>
       <c r="D9" s="123" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E9" s="123" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F9" s="123" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G9" s="123" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="162" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B10" s="173"/>
       <c r="C10" s="177" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D10" s="176" t="str">
         <f aca="false">A7</f>
@@ -12906,11 +12989,11 @@
     </row>
     <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="162" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B11" s="173"/>
       <c r="C11" s="177" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D11" s="176" t="str">
         <f aca="false">A11</f>
@@ -12938,11 +13021,11 @@
     </row>
     <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="162" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B12" s="173"/>
       <c r="C12" s="177" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D12" s="193" t="str">
         <f aca="false">A15</f>
@@ -12970,11 +13053,11 @@
     </row>
     <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="162" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B13" s="173"/>
       <c r="C13" s="177" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D13" s="176" t="str">
         <f aca="false">A19</f>
@@ -13002,11 +13085,11 @@
     </row>
     <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="162" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B14" s="173"/>
       <c r="C14" s="177" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D14" s="176" t="str">
         <f aca="false">A23</f>
@@ -13034,11 +13117,11 @@
     </row>
     <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="162" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B15" s="173"/>
       <c r="C15" s="177" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D15" s="195" t="s">
         <v>63</v>
@@ -13064,11 +13147,11 @@
     </row>
     <row r="16" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="162" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B16" s="178"/>
       <c r="C16" s="179" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D16" s="180"/>
       <c r="E16" s="181"/>
@@ -13077,32 +13160,32 @@
     </row>
     <row r="17" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="162" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B17" s="173"/>
       <c r="C17" s="187"/>
       <c r="D17" s="197" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E17" s="197" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F17" s="198" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="G17" s="199"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="162" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B18" s="173"/>
       <c r="C18" s="187"/>
       <c r="D18" s="123" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E18" s="123" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F18" s="200" t="s">
         <v>63</v>
@@ -13111,11 +13194,11 @@
     </row>
     <row r="19" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="162" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B19" s="173"/>
       <c r="C19" s="174" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D19" s="191" t="str">
         <f aca="false">A29</f>
@@ -13133,11 +13216,11 @@
     </row>
     <row r="20" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="162" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B20" s="173"/>
       <c r="C20" s="174" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D20" s="191" t="str">
         <f aca="false">A32</f>
@@ -13155,11 +13238,11 @@
     </row>
     <row r="21" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="162" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B21" s="173"/>
       <c r="C21" s="174" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D21" s="191" t="str">
         <f aca="false">A35</f>
@@ -13177,11 +13260,11 @@
     </row>
     <row r="22" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="162" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B22" s="173"/>
       <c r="C22" s="174" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D22" s="191" t="str">
         <f aca="false">A38</f>
@@ -13199,11 +13282,11 @@
     </row>
     <row r="23" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="162" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B23" s="173"/>
       <c r="C23" s="174" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D23" s="191" t="str">
         <f aca="false">A41</f>
@@ -13221,11 +13304,11 @@
     </row>
     <row r="24" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="162" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B24" s="173"/>
       <c r="C24" s="174" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D24" s="191" t="str">
         <f aca="false">A44</f>
@@ -13243,11 +13326,11 @@
     </row>
     <row r="25" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="162" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B25" s="173"/>
       <c r="C25" s="174" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D25" s="191" t="str">
         <f aca="false">A47</f>
@@ -13265,11 +13348,11 @@
     </row>
     <row r="26" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="162" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B26" s="173"/>
       <c r="C26" s="174" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D26" s="191" t="str">
         <f aca="false">A50</f>
@@ -13287,11 +13370,11 @@
     </row>
     <row r="27" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="162" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B27" s="170"/>
       <c r="C27" s="171" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D27" s="172"/>
       <c r="E27" s="172"/>
@@ -13300,11 +13383,11 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="162" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B28" s="173"/>
       <c r="C28" s="177" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D28" s="202" t="str">
         <f aca="false">A54</f>
@@ -13316,7 +13399,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="162" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B29" s="203"/>
       <c r="C29" s="186"/>
@@ -13327,66 +13410,66 @@
     </row>
     <row r="30" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="162" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B30" s="173"/>
       <c r="C30" s="206"/>
       <c r="D30" s="207" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E30" s="188" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F30" s="188" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="G30" s="188" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="162" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B31" s="173"/>
       <c r="C31" s="206"/>
       <c r="D31" s="208" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E31" s="197" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F31" s="197" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="G31" s="197"/>
     </row>
     <row r="32" customFormat="false" ht="13.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="162" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B32" s="173"/>
       <c r="C32" s="206"/>
       <c r="D32" s="209" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E32" s="123" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F32" s="123" t="s">
         <v>63</v>
       </c>
       <c r="G32" s="210" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="162" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B33" s="173"/>
       <c r="C33" s="177" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D33" s="211" t="str">
         <f aca="false">A55</f>
@@ -13407,11 +13490,11 @@
     </row>
     <row r="34" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="162" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B34" s="173"/>
       <c r="C34" s="177" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D34" s="211" t="str">
         <f aca="false">A59</f>
@@ -13430,11 +13513,11 @@
     </row>
     <row r="35" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="162" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B35" s="203"/>
       <c r="C35" s="215" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D35" s="216" t="str">
         <f aca="false">A61</f>
@@ -13453,11 +13536,11 @@
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="162" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B36" s="173"/>
       <c r="C36" s="219" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D36" s="219"/>
       <c r="E36" s="220" t="str">
@@ -13469,11 +13552,11 @@
     </row>
     <row r="37" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="162" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B37" s="170"/>
       <c r="C37" s="171" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D37" s="172"/>
       <c r="E37" s="172"/>
@@ -13482,11 +13565,11 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="162" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B38" s="173"/>
       <c r="C38" s="174" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D38" s="221" t="str">
         <f aca="false">A65</f>
@@ -13498,7 +13581,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="162" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B39" s="173"/>
       <c r="C39" s="204"/>
@@ -13509,43 +13592,43 @@
     </row>
     <row r="40" customFormat="false" ht="19.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="162" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B40" s="223"/>
       <c r="C40" s="224"/>
       <c r="D40" s="188" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E40" s="225" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F40" s="188" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="G40" s="188" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="162" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B41" s="173"/>
       <c r="C41" s="187"/>
       <c r="D41" s="197" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E41" s="226" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="F41" s="197"/>
       <c r="G41" s="197" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="162" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B42" s="173"/>
       <c r="C42" s="227"/>
@@ -13564,11 +13647,11 @@
     </row>
     <row r="43" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="162" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B43" s="173"/>
       <c r="C43" s="174" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D43" s="229" t="str">
         <f aca="false">A66</f>
@@ -13589,11 +13672,11 @@
     </row>
     <row r="44" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="162" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B44" s="173"/>
       <c r="C44" s="174" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D44" s="229" t="str">
         <f aca="false">A70</f>
@@ -13614,11 +13697,11 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="162" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B45" s="173"/>
       <c r="C45" s="230" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D45" s="231"/>
       <c r="E45" s="231"/>
@@ -13627,11 +13710,11 @@
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="162" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B46" s="173"/>
       <c r="C46" s="230" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D46" s="174"/>
       <c r="E46" s="174"/>
@@ -13640,7 +13723,7 @@
     </row>
     <row r="47" customFormat="false" ht="6.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="162" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B47" s="173"/>
       <c r="C47" s="232"/>
@@ -13652,30 +13735,30 @@
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="162" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B48" s="173"/>
       <c r="C48" s="187"/>
       <c r="D48" s="188" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E48" s="188" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="F48" s="235"/>
       <c r="G48" s="205"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="162" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B49" s="173"/>
       <c r="C49" s="187"/>
       <c r="D49" s="123" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E49" s="123" t="s">
-        <v>219</v>
+        <v>61</v>
       </c>
       <c r="F49" s="235"/>
       <c r="G49" s="205"/>
@@ -14621,8 +14704,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ113"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14697,7 +14780,7 @@
       </c>
       <c r="B3" s="256"/>
       <c r="C3" s="257" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D3" s="258"/>
       <c r="E3" s="258"/>
@@ -14710,7 +14793,7 @@
       </c>
       <c r="B4" s="173"/>
       <c r="C4" s="260" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D4" s="261" t="str">
         <f aca="false">A3</f>
@@ -14722,7 +14805,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="162" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B5" s="173"/>
       <c r="C5" s="260"/>
@@ -14748,7 +14831,7 @@
       </c>
       <c r="B7" s="173"/>
       <c r="C7" s="264" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D7" s="265" t="str">
         <f aca="false">A4</f>
@@ -14807,7 +14890,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="162" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B11" s="256"/>
       <c r="C11" s="257" t="s">
@@ -14820,7 +14903,7 @@
     </row>
     <row r="12" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="162" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B12" s="173"/>
       <c r="C12" s="204"/>
@@ -14850,7 +14933,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="162" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B14" s="173"/>
       <c r="C14" s="187"/>
@@ -14867,7 +14950,7 @@
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="162" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B15" s="203"/>
       <c r="C15" s="273"/>
@@ -14886,7 +14969,7 @@
     </row>
     <row r="16" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="162" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B16" s="173"/>
       <c r="C16" s="187"/>
@@ -14901,7 +14984,7 @@
       </c>
       <c r="B17" s="173"/>
       <c r="C17" s="274" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D17" s="243" t="str">
         <f aca="false">A7</f>
@@ -14922,11 +15005,11 @@
     </row>
     <row r="18" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="162" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B18" s="173"/>
       <c r="C18" s="274" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D18" s="243" t="str">
         <f aca="false">A11</f>
@@ -14947,11 +15030,11 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="162" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B19" s="173"/>
       <c r="C19" s="274" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D19" s="243" t="str">
         <f aca="false">A15</f>
@@ -14972,11 +15055,11 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="162" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B20" s="173"/>
       <c r="C20" s="274" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D20" s="243" t="str">
         <f aca="false">A19</f>
@@ -15022,7 +15105,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="162" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B22" s="173"/>
       <c r="C22" s="267" t="s">
@@ -15044,7 +15127,7 @@
     </row>
     <row r="23" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="162" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B23" s="173"/>
       <c r="C23" s="204"/>
@@ -15055,7 +15138,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="162" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B24" s="256"/>
       <c r="C24" s="257" t="s">
@@ -15079,7 +15162,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="162" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B26" s="173"/>
       <c r="C26" s="187"/>
@@ -15094,7 +15177,7 @@
     </row>
     <row r="27" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="162" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B27" s="173"/>
       <c r="C27" s="187"/>
@@ -15105,7 +15188,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="162" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B28" s="173"/>
       <c r="C28" s="281" t="s">
@@ -15124,7 +15207,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="162" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B29" s="173"/>
       <c r="C29" s="281" t="s">
@@ -15162,7 +15245,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="162" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B31" s="173"/>
       <c r="C31" s="281" t="s">
@@ -15575,7 +15658,7 @@
       </c>
       <c r="B56" s="173"/>
       <c r="C56" s="174" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D56" s="174"/>
       <c r="E56" s="243" t="str">
@@ -18282,7 +18365,7 @@
         <v>497</v>
       </c>
       <c r="B2" s="370" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C2" s="370"/>
       <c r="D2" s="370"/>
@@ -20096,7 +20179,7 @@
   </sheetPr>
   <dimension ref="A1:Q140"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B4" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B4" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
AE-961 add last page swedish translations to xlsx template
</commit_message>
<xml_diff>
--- a/etp-backend/src/main/resources/energiatodistus-2018-sv.xlsx
+++ b/etp-backend/src/main/resources/energiatodistus-2018-sv.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="1) etusivu" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,23 +19,23 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'1) etusivu'!$B$1:$R$51</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$59</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$58</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area" vbProcedure="false">'3) E-luvun laskennan lähtöt.'!$B$2:$G$67</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$1:$G$78</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$2:$G$77</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area" vbProcedure="false">'5) toteutunut kulutus'!$B$2:$K$55</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm.Print_Area" vbProcedure="false">'6) huomiot 1'!$B$2:$F$53</definedName>
-    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$61</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$60</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area" vbProcedure="false">'8) lisämerkintöjä'!$B$1:$M$63</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'1) etusivu'!$B$1:$R$50</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'2) E-luokka'!$B$2:$K$59</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$58</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$59</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'3) E-luvun laskennan lähtöt.'!$B$2:$G$66</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$2:$G$76</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$2:$G$77</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$1:$G$78</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'5) toteutunut kulutus'!$B$2:$L$54</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'6) huomiot 1'!$B$2:$G$52</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'7) huomiot 2'!$B$2:$G$59</definedName>
-    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$60</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$61</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="761">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="760">
   <si>
     <t xml:space="preserve">[:id]</t>
   </si>
@@ -339,6 +339,7 @@
         <color rgb="FF009EE0"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">E</t>
     </r>
@@ -1454,6 +1455,7 @@
         <color rgb="FF009EE0"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
     </r>
@@ -1581,60 +1583,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF009EE0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">kWh</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="10"/>
-        <color rgb="FF009EE0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">E</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF009EE0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">/(m</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <color rgb="FF009EE0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF009EE0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">år)</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">[:tulokset :kaytettavat-energiamuodot :fossiilinen-polttoaine-kertoimella]</t>
   </si>
   <si>
@@ -3026,7 +2974,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">rak omin</t>
+      <t xml:space="preserve">byg spec</t>
     </r>
     <r>
       <rPr>
@@ -3036,7 +2984,16 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">, Wh/m^2^K</t>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF009EE0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Wh/m²K</t>
     </r>
   </si>
   <si>
@@ -3068,7 +3025,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">sp</t>
+      <t xml:space="preserve">ib</t>
     </r>
     <r>
       <rPr>
@@ -3087,28 +3044,28 @@
   <si>
     <r>
       <rPr>
-        <sz val="8"/>
+        <sz val="9"/>
         <color rgb="FF009EE0"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Andelen värmeenergi som värmepumpen alstrar jämfört med den värmeenergi som behövs för uppvärmning av utrymmen  Q</t>
+      <t xml:space="preserve">Andelen värmeenergi som värmepumpen alstrar den värmeenergi som behövs för uppvärmning av utrymmen Q</t>
     </r>
     <r>
       <rPr>
         <vertAlign val="subscript"/>
-        <sz val="8"/>
+        <sz val="9"/>
         <color rgb="FF009EE0"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">LP</t>
+      <t xml:space="preserve">VP</t>
     </r>
     <r>
       <rPr>
-        <sz val="8"/>
+        <sz val="9"/>
         <color rgb="FF009EE0"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -3119,17 +3076,17 @@
     <r>
       <rPr>
         <vertAlign val="subscript"/>
-        <sz val="8"/>
+        <sz val="9"/>
         <color rgb="FF009EE0"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">lämmitys, tilat</t>
+      <t xml:space="preserve">uppvärmning, utrymmen</t>
     </r>
     <r>
       <rPr>
-        <sz val="8"/>
+        <sz val="9"/>
         <color rgb="FF009EE0"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -3144,28 +3101,28 @@
   <si>
     <r>
       <rPr>
-        <sz val="8"/>
+        <sz val="9"/>
         <color rgb="FF009EE0"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Andelen värmeenergi som värmepumpen alstrar jämfört med den värmeenergi som behövs för uppvärmning av tappvatten Q</t>
+      <t xml:space="preserve">Andelen värmeenergi som värmepumpen alstrar den värmeenergi som behövs för uppvärmning av tappvatten Q</t>
     </r>
     <r>
       <rPr>
         <vertAlign val="subscript"/>
-        <sz val="8"/>
+        <sz val="9"/>
         <color rgb="FF009EE0"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">LP</t>
+      <t xml:space="preserve">VP</t>
     </r>
     <r>
       <rPr>
-        <sz val="8"/>
+        <sz val="9"/>
         <color rgb="FF009EE0"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -3176,13 +3133,13 @@
     <r>
       <rPr>
         <vertAlign val="subscript"/>
-        <sz val="8"/>
+        <sz val="9"/>
         <color rgb="FF009EE0"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">lämmitys, lkv</t>
+      <t xml:space="preserve">uppvärmning, vtv</t>
     </r>
   </si>
   <si>
@@ -3208,7 +3165,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">jakelu, ulos</t>
+      <t xml:space="preserve">distribution, ut</t>
     </r>
     <r>
       <rPr>
@@ -3609,13 +3566,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <vertAlign val="subscript"/>
-      <sz val="10"/>
-      <color rgb="FF009EE0"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -3753,13 +3703,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <vertAlign val="superscript"/>
-      <sz val="10"/>
-      <color rgb="FF009EE0"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b val="true"/>
       <vertAlign val="subscript"/>
       <sz val="10"/>
@@ -3841,8 +3784,21 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF009EE0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF009EE0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <vertAlign val="subscript"/>
-      <sz val="8"/>
+      <sz val="9"/>
       <color rgb="FF009EE0"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -4692,11 +4648,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4704,35 +4660,35 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="24" fillId="4" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="23" fillId="4" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="24" fillId="5" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="23" fillId="5" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="24" fillId="6" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="23" fillId="6" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="24" fillId="7" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="23" fillId="7" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="24" fillId="8" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="23" fillId="8" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="24" fillId="9" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="23" fillId="9" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4740,15 +4696,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="24" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="23" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4756,11 +4712,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4804,19 +4760,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4904,7 +4860,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="3" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="28" fillId="3" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4940,7 +4896,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -4988,43 +4944,43 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="173" fontId="4" fillId="0" borderId="14" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="32" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="173" fontId="4" fillId="0" borderId="14" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -5048,11 +5004,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="34" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="34" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -5068,7 +5024,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -5076,11 +5032,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -5108,7 +5064,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="34" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -5124,7 +5080,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -5148,7 +5104,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5232,7 +5188,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -5256,7 +5212,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="24" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="23" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -5300,15 +5256,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="43" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="169" fontId="41" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="42" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="40" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -5324,7 +5280,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5364,7 +5320,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5408,7 +5364,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="23" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5484,7 +5440,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="44" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="42" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5508,7 +5464,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="35" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -5556,11 +5512,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="45" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="43" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="45" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="43" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5576,11 +5532,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5596,7 +5552,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="46" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="44" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5620,7 +5576,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5704,7 +5660,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5724,7 +5680,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="47" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="45" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -5736,7 +5692,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="48" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="46" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5752,7 +5708,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="49" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="47" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -5768,7 +5724,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="49" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -8168,9 +8124,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>229320</xdr:colOff>
+      <xdr:colOff>228960</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>243720</xdr:rowOff>
+      <xdr:rowOff>243360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8184,7 +8140,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="4656960"/>
-          <a:ext cx="739440" cy="196200"/>
+          <a:ext cx="739080" cy="195840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8205,9 +8161,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>129240</xdr:colOff>
+      <xdr:colOff>128880</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>243720</xdr:rowOff>
+      <xdr:rowOff>243360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8221,7 +8177,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="4971240"/>
-          <a:ext cx="1082880" cy="196200"/>
+          <a:ext cx="1082520" cy="195840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8242,9 +8198,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2520</xdr:colOff>
+      <xdr:colOff>2160</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>243720</xdr:rowOff>
+      <xdr:rowOff>243360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8258,7 +8214,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="5285520"/>
-          <a:ext cx="1389600" cy="196200"/>
+          <a:ext cx="1389240" cy="195840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8279,9 +8235,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>326520</xdr:colOff>
+      <xdr:colOff>326160</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>243720</xdr:rowOff>
+      <xdr:rowOff>243360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8295,7 +8251,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="5599800"/>
-          <a:ext cx="1713600" cy="196200"/>
+          <a:ext cx="1713240" cy="195840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8316,9 +8272,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>199800</xdr:colOff>
+      <xdr:colOff>199440</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>256680</xdr:rowOff>
+      <xdr:rowOff>256320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8332,7 +8288,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="5909760"/>
-          <a:ext cx="2020680" cy="209160"/>
+          <a:ext cx="2020320" cy="208800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8353,9 +8309,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>142920</xdr:colOff>
+      <xdr:colOff>142560</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>243720</xdr:rowOff>
+      <xdr:rowOff>243360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8369,7 +8325,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="6219720"/>
-          <a:ext cx="2356920" cy="196200"/>
+          <a:ext cx="2356560" cy="195840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8390,9 +8346,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>83160</xdr:colOff>
+      <xdr:colOff>82800</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>244800</xdr:rowOff>
+      <xdr:rowOff>244440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -8402,7 +8358,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="6531480"/>
-          <a:ext cx="2669760" cy="195120"/>
+          <a:ext cx="2669400" cy="194760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8771,9 +8727,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>282600</xdr:colOff>
+      <xdr:colOff>282240</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>83880</xdr:rowOff>
+      <xdr:rowOff>83520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -8783,7 +8739,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1978200" y="78480"/>
-          <a:ext cx="6968880" cy="10490400"/>
+          <a:ext cx="6968520" cy="10490040"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -12759,8 +12715,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ92"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G45" activeCellId="0" sqref="G45"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G57" activeCellId="0" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14964,7 +14920,7 @@
         <v>288</v>
       </c>
       <c r="G15" s="200" t="s">
-        <v>289</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14980,7 +14936,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="162" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B17" s="173"/>
       <c r="C17" s="274" t="s">
@@ -15080,11 +15036,11 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="162" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B21" s="173"/>
       <c r="C21" s="276" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D21" s="243" t="str">
         <f aca="false">A23</f>
@@ -15109,7 +15065,7 @@
       </c>
       <c r="B22" s="173"/>
       <c r="C22" s="267" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D22" s="277" t="str">
         <f aca="false">A42</f>
@@ -15142,7 +15098,7 @@
       </c>
       <c r="B24" s="256"/>
       <c r="C24" s="257" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D24" s="172"/>
       <c r="E24" s="258"/>
@@ -15151,7 +15107,7 @@
     </row>
     <row r="25" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="162" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B25" s="223"/>
       <c r="C25" s="279"/>
@@ -15192,7 +15148,7 @@
       </c>
       <c r="B28" s="173"/>
       <c r="C28" s="281" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D28" s="281"/>
       <c r="E28" s="243" t="str">
@@ -15211,7 +15167,7 @@
       </c>
       <c r="B29" s="173"/>
       <c r="C29" s="281" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D29" s="281"/>
       <c r="E29" s="243" t="str">
@@ -15226,11 +15182,11 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="162" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B30" s="173"/>
       <c r="C30" s="281" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D30" s="281"/>
       <c r="E30" s="243" t="str">
@@ -15249,7 +15205,7 @@
       </c>
       <c r="B31" s="173"/>
       <c r="C31" s="281" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D31" s="281"/>
       <c r="E31" s="243" t="str">
@@ -15264,11 +15220,11 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="162" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B32" s="173"/>
       <c r="C32" s="281" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D32" s="281"/>
       <c r="E32" s="243" t="str">
@@ -15283,11 +15239,11 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="162" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B33" s="173"/>
       <c r="C33" s="281" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D33" s="281"/>
       <c r="E33" s="243" t="str">
@@ -15302,7 +15258,7 @@
     </row>
     <row r="34" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="162" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B34" s="203"/>
       <c r="C34" s="269"/>
@@ -15313,11 +15269,11 @@
     </row>
     <row r="35" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="162" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B35" s="256"/>
       <c r="C35" s="257" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D35" s="258"/>
       <c r="E35" s="258"/>
@@ -15326,7 +15282,7 @@
     </row>
     <row r="36" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="162" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B36" s="173"/>
       <c r="C36" s="204"/>
@@ -15337,24 +15293,24 @@
     </row>
     <row r="37" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="162" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B37" s="173"/>
       <c r="C37" s="187"/>
       <c r="D37" s="187"/>
       <c r="E37" s="197" t="s">
+        <v>309</v>
+      </c>
+      <c r="F37" s="197" t="s">
         <v>310</v>
       </c>
-      <c r="F37" s="197" t="s">
+      <c r="G37" s="197" t="s">
         <v>311</v>
-      </c>
-      <c r="G37" s="197" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="162" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B38" s="173"/>
       <c r="C38" s="187"/>
@@ -15371,7 +15327,7 @@
     </row>
     <row r="39" customFormat="false" ht="6.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="162" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B39" s="173"/>
       <c r="C39" s="187"/>
@@ -15382,7 +15338,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="162" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B40" s="173"/>
       <c r="C40" s="174" t="s">
@@ -15395,11 +15351,11 @@
     </row>
     <row r="41" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="162" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B41" s="173"/>
       <c r="C41" s="174" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D41" s="174"/>
       <c r="E41" s="243" t="str">
@@ -15416,11 +15372,11 @@
     </row>
     <row r="42" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="162" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B42" s="173"/>
       <c r="C42" s="174" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D42" s="174"/>
       <c r="E42" s="243" t="str">
@@ -15437,11 +15393,11 @@
     </row>
     <row r="43" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="162" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B43" s="173"/>
       <c r="C43" s="174" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D43" s="174"/>
       <c r="E43" s="243" t="str">
@@ -15458,11 +15414,11 @@
     </row>
     <row r="44" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="162" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B44" s="173"/>
       <c r="C44" s="174" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D44" s="174"/>
       <c r="E44" s="243" t="str">
@@ -15478,7 +15434,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="162" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B45" s="173"/>
       <c r="C45" s="174" t="s">
@@ -15500,11 +15456,11 @@
     </row>
     <row r="46" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="162" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B46" s="173"/>
       <c r="C46" s="174" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D46" s="174"/>
       <c r="E46" s="243" t="str">
@@ -15520,11 +15476,11 @@
     </row>
     <row r="47" customFormat="false" ht="20.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="162" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B47" s="173"/>
       <c r="C47" s="267" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D47" s="267"/>
       <c r="E47" s="285" t="str">
@@ -15542,11 +15498,11 @@
     </row>
     <row r="48" customFormat="false" ht="19.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="162" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B48" s="173"/>
       <c r="C48" s="230" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D48" s="267"/>
       <c r="E48" s="237"/>
@@ -15555,7 +15511,7 @@
     </row>
     <row r="49" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="162" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B49" s="173"/>
       <c r="C49" s="204"/>
@@ -15566,11 +15522,11 @@
     </row>
     <row r="50" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="162" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B50" s="256"/>
       <c r="C50" s="257" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D50" s="258"/>
       <c r="E50" s="258"/>
@@ -15579,7 +15535,7 @@
     </row>
     <row r="51" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="162" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B51" s="173"/>
       <c r="C51" s="204"/>
@@ -15590,7 +15546,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="162" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B52" s="173"/>
       <c r="C52" s="187"/>
@@ -15605,7 +15561,7 @@
     </row>
     <row r="53" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="162" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B53" s="173"/>
       <c r="C53" s="187"/>
@@ -15616,11 +15572,11 @@
     </row>
     <row r="54" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="162" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B54" s="173"/>
       <c r="C54" s="174" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D54" s="174"/>
       <c r="E54" s="243" t="str">
@@ -15635,11 +15591,11 @@
     </row>
     <row r="55" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="162" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B55" s="173"/>
       <c r="C55" s="174" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D55" s="174"/>
       <c r="E55" s="243" t="str">
@@ -15654,7 +15610,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="162" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B56" s="173"/>
       <c r="C56" s="174" t="s">
@@ -15673,11 +15629,11 @@
     </row>
     <row r="57" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="162" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B57" s="173"/>
       <c r="C57" s="174" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D57" s="174"/>
       <c r="E57" s="243" t="str">
@@ -15692,7 +15648,7 @@
     </row>
     <row r="58" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="162" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B58" s="173"/>
       <c r="C58" s="174"/>
@@ -15703,11 +15659,11 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="162" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B59" s="173"/>
       <c r="C59" s="230" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D59" s="288"/>
       <c r="E59" s="289"/>
@@ -15716,11 +15672,11 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="162" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B60" s="173"/>
       <c r="C60" s="230" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D60" s="288"/>
       <c r="E60" s="290"/>
@@ -15729,7 +15685,7 @@
     </row>
     <row r="61" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="162" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B61" s="173"/>
       <c r="C61" s="174"/>
@@ -15740,11 +15696,11 @@
     </row>
     <row r="62" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="162" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B62" s="256"/>
       <c r="C62" s="257" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D62" s="258"/>
       <c r="E62" s="258"/>
@@ -15753,7 +15709,7 @@
     </row>
     <row r="63" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="162" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B63" s="173"/>
       <c r="C63" s="204"/>
@@ -15764,7 +15720,7 @@
     </row>
     <row r="64" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="162" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B64" s="173"/>
       <c r="C64" s="187"/>
@@ -15779,7 +15735,7 @@
     </row>
     <row r="65" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="162" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B65" s="173"/>
       <c r="C65" s="187"/>
@@ -15790,11 +15746,11 @@
     </row>
     <row r="66" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="162" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B66" s="173"/>
       <c r="C66" s="174" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D66" s="174"/>
       <c r="E66" s="243" t="str">
@@ -15809,7 +15765,7 @@
     </row>
     <row r="67" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="162" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B67" s="173"/>
       <c r="C67" s="174" t="s">
@@ -15828,7 +15784,7 @@
     </row>
     <row r="68" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="162" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B68" s="173"/>
       <c r="C68" s="174" t="s">
@@ -15847,7 +15803,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="162" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B69" s="173"/>
       <c r="C69" s="174" t="s">
@@ -15866,11 +15822,11 @@
     </row>
     <row r="70" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="162" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B70" s="173"/>
       <c r="C70" s="174" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D70" s="174"/>
       <c r="E70" s="243" t="str">
@@ -15885,7 +15841,7 @@
     </row>
     <row r="71" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="162" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B71" s="173"/>
       <c r="C71" s="174"/>
@@ -15896,11 +15852,11 @@
     </row>
     <row r="72" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="162" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B72" s="256"/>
       <c r="C72" s="257" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D72" s="258"/>
       <c r="E72" s="258"/>
@@ -15909,7 +15865,7 @@
     </row>
     <row r="73" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="162" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B73" s="173"/>
       <c r="C73" s="204"/>
@@ -15920,11 +15876,11 @@
     </row>
     <row r="74" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="162" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B74" s="173"/>
       <c r="C74" s="174" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D74" s="174"/>
       <c r="E74" s="292" t="str">
@@ -15936,7 +15892,7 @@
     </row>
     <row r="75" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="162" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B75" s="247"/>
       <c r="C75" s="185"/>
@@ -15947,12 +15903,12 @@
     </row>
     <row r="76" customFormat="false" ht="5.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="162" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="162" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B77" s="294" t="str">
         <f aca="false">"Certifikatbeteckning: "&amp;A1&amp;", 4/8"</f>
@@ -15966,182 +15922,182 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="162" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="162" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="162" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="162" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="162" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="162" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="162" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="162" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="162" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="162" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="162" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="162" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="162" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="162" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="162" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="162" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="162" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="162" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="162" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="162" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="162" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="162" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="162" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="162" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="162" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="162" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="162" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="162" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="162" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="162" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="162" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="162" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="162" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="162" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="162" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="162" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
   </sheetData>
@@ -16623,11 +16579,11 @@
     </row>
     <row r="2" s="300" customFormat="true" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="295" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B2" s="296"/>
       <c r="C2" s="297" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D2" s="297"/>
       <c r="E2" s="297"/>
@@ -16686,11 +16642,11 @@
     </row>
     <row r="3" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="99" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B3" s="107"/>
       <c r="C3" s="301" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D3" s="301"/>
       <c r="E3" s="301"/>
@@ -16703,7 +16659,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="99" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B4" s="107"/>
       <c r="C4" s="70"/>
@@ -16718,11 +16674,11 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="99" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B5" s="103"/>
       <c r="C5" s="104" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D5" s="104"/>
       <c r="E5" s="104"/>
@@ -16735,7 +16691,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="99" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B6" s="107"/>
       <c r="C6" s="0"/>
@@ -16751,7 +16707,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="99" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B7" s="107"/>
       <c r="C7" s="116" t="s">
@@ -16762,7 +16718,7 @@
         <v>#function[solita.etp.service.energiatodistus-pdf/fn--61283]</v>
       </c>
       <c r="E7" s="303" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F7" s="112"/>
       <c r="G7" s="304"/>
@@ -16774,7 +16730,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="99" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B8" s="107"/>
       <c r="C8" s="6"/>
@@ -16789,7 +16745,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="99" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B9" s="115"/>
       <c r="C9" s="117"/>
@@ -16804,11 +16760,11 @@
     </row>
     <row r="10" s="300" customFormat="true" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="295" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B10" s="306"/>
       <c r="C10" s="307" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D10" s="308"/>
       <c r="E10" s="308"/>
@@ -16871,7 +16827,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="99" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B11" s="107"/>
       <c r="C11" s="6"/>
@@ -16886,11 +16842,11 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="99" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B12" s="107"/>
       <c r="C12" s="110" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D12" s="110"/>
       <c r="E12" s="110"/>
@@ -16909,7 +16865,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="99" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B13" s="107"/>
       <c r="C13" s="110"/>
@@ -16924,11 +16880,11 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="99" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B14" s="107"/>
       <c r="C14" s="110" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D14" s="110"/>
       <c r="E14" s="110"/>
@@ -16947,7 +16903,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="99" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B15" s="107"/>
       <c r="C15" s="110"/>
@@ -16962,11 +16918,11 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="99" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B16" s="107"/>
       <c r="C16" s="321" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D16" s="110"/>
       <c r="E16" s="110"/>
@@ -16985,11 +16941,11 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="99" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B17" s="107"/>
       <c r="C17" s="321" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D17" s="110"/>
       <c r="E17" s="110"/>
@@ -17008,7 +16964,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="99" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B18" s="107"/>
       <c r="C18" s="321"/>
@@ -17023,11 +16979,11 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="99" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B19" s="107"/>
       <c r="C19" s="110" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D19" s="110"/>
       <c r="E19" s="110"/>
@@ -17046,7 +17002,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="99" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B20" s="115"/>
       <c r="C20" s="322"/>
@@ -17061,22 +17017,22 @@
     </row>
     <row r="21" s="300" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="295" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B21" s="306"/>
       <c r="C21" s="307" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D21" s="307"/>
       <c r="E21" s="307"/>
       <c r="F21" s="326" t="s">
+        <v>434</v>
+      </c>
+      <c r="G21" s="327" t="s">
         <v>435</v>
       </c>
-      <c r="G21" s="327" t="s">
+      <c r="H21" s="326" t="s">
         <v>436</v>
-      </c>
-      <c r="H21" s="326" t="s">
-        <v>437</v>
       </c>
       <c r="I21" s="327" t="s">
         <v>61</v>
@@ -17134,7 +17090,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="99" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B22" s="101"/>
       <c r="C22" s="328"/>
@@ -17149,11 +17105,11 @@
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="99" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B23" s="107"/>
       <c r="C23" s="110" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D23" s="110"/>
       <c r="E23" s="110"/>
@@ -17162,7 +17118,7 @@
         <v>[:toteutunut-ostoenergiankulutus :ostetut-polttoaineet :kevyt-polttooljy]</v>
       </c>
       <c r="G23" s="335" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H23" s="336" t="n">
         <v>10</v>
@@ -17179,11 +17135,11 @@
     </row>
     <row r="24" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="99" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B24" s="107"/>
       <c r="C24" s="110" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D24" s="110"/>
       <c r="E24" s="110"/>
@@ -17192,7 +17148,7 @@
         <v>[:toteutunut-ostoenergiankulutus :ostetut-polttoaineet :pilkkeet-havu-sekapuu]</v>
       </c>
       <c r="G24" s="335" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="H24" s="336" t="n">
         <v>1300</v>
@@ -17209,11 +17165,11 @@
     </row>
     <row r="25" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="99" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B25" s="107"/>
       <c r="C25" s="110" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D25" s="110"/>
       <c r="E25" s="110"/>
@@ -17222,7 +17178,7 @@
         <v>[:toteutunut-ostoenergiankulutus :ostetut-polttoaineet :pilkkeet-koivu]</v>
       </c>
       <c r="G25" s="335" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="H25" s="336" t="n">
         <v>1700</v>
@@ -17239,11 +17195,11 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="99" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B26" s="107"/>
       <c r="C26" s="110" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D26" s="110"/>
       <c r="E26" s="110"/>
@@ -17252,7 +17208,7 @@
         <v>[:toteutunut-ostoenergiankulutus :ostetut-polttoaineet :puupelletit]</v>
       </c>
       <c r="G26" s="335" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="H26" s="336" t="n">
         <v>4.7</v>
@@ -17269,7 +17225,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="99" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B27" s="107"/>
       <c r="C27" s="337" t="str">
@@ -17302,7 +17258,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="99" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B28" s="107"/>
       <c r="C28" s="337" t="str">
@@ -17335,11 +17291,11 @@
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="99" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B29" s="107"/>
       <c r="C29" s="340" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D29" s="340"/>
       <c r="E29" s="340"/>
@@ -17352,7 +17308,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="99" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B30" s="107"/>
       <c r="C30" s="340"/>
@@ -17367,7 +17323,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="99" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B31" s="107"/>
       <c r="C31" s="340"/>
@@ -17382,7 +17338,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="99" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B32" s="107"/>
       <c r="C32" s="340"/>
@@ -17397,7 +17353,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="99" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B33" s="107"/>
       <c r="C33" s="344"/>
@@ -17412,7 +17368,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="99" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B34" s="115"/>
       <c r="C34" s="345"/>
@@ -17427,11 +17383,11 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="99" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B35" s="107"/>
       <c r="C35" s="307" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D35" s="307"/>
       <c r="E35" s="307"/>
@@ -17444,7 +17400,7 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="99" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B36" s="107"/>
       <c r="C36" s="307"/>
@@ -17463,7 +17419,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="99" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B37" s="101"/>
       <c r="C37" s="351"/>
@@ -17478,11 +17434,11 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="99" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B38" s="107"/>
       <c r="C38" s="34" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D38" s="34"/>
       <c r="E38" s="34"/>
@@ -17501,7 +17457,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="99" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B39" s="107"/>
       <c r="C39" s="34"/>
@@ -17516,11 +17472,11 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="99" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B40" s="107"/>
       <c r="C40" s="34" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D40" s="34"/>
       <c r="E40" s="34"/>
@@ -17539,7 +17495,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="99" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B41" s="107"/>
       <c r="C41" s="34"/>
@@ -17554,11 +17510,11 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="99" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B42" s="107"/>
       <c r="C42" s="34" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D42" s="34"/>
       <c r="E42" s="34"/>
@@ -17577,7 +17533,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="99" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B43" s="107"/>
       <c r="C43" s="34"/>
@@ -17592,11 +17548,11 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="99" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B44" s="107"/>
       <c r="C44" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D44" s="34"/>
       <c r="E44" s="34"/>
@@ -17615,7 +17571,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="99" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B45" s="107"/>
       <c r="C45" s="34"/>
@@ -17630,11 +17586,11 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="99" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B46" s="107"/>
       <c r="C46" s="18" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D46" s="18"/>
       <c r="E46" s="18"/>
@@ -17653,7 +17609,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="99" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B47" s="115"/>
       <c r="C47" s="363"/>
@@ -17668,11 +17624,11 @@
     </row>
     <row r="48" customFormat="false" ht="19.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="99" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B48" s="101"/>
       <c r="C48" s="366" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D48" s="366"/>
       <c r="E48" s="366"/>
@@ -17685,7 +17641,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="99" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B49" s="107"/>
       <c r="C49" s="366"/>
@@ -17700,7 +17656,7 @@
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="99" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B50" s="107"/>
       <c r="C50" s="366"/>
@@ -17715,7 +17671,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="99" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B51" s="107"/>
       <c r="C51" s="366"/>
@@ -17730,7 +17686,7 @@
     </row>
     <row r="52" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="99" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B52" s="107"/>
       <c r="C52" s="366"/>
@@ -17745,7 +17701,7 @@
     </row>
     <row r="53" customFormat="false" ht="33.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="99" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B53" s="154"/>
       <c r="C53" s="366"/>
@@ -17761,7 +17717,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="99" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B54" s="368" t="str">
         <f aca="false">"Certifikatbeteckning: "&amp;A1&amp;", 5/8"</f>
@@ -17779,7 +17735,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="99" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B55" s="368"/>
       <c r="C55" s="368"/>
@@ -17794,62 +17750,62 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="99" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="99" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="99" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="99" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="99" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="99" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="99" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="99" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="99" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="99" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="99" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="99" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
   </sheetData>
@@ -18362,7 +18318,7 @@
     </row>
     <row r="2" s="371" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="251" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B2" s="370" t="s">
         <v>99</v>
@@ -18404,10 +18360,10 @@
     </row>
     <row r="3" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="162" t="s">
+        <v>497</v>
+      </c>
+      <c r="B3" s="372" t="s">
         <v>498</v>
-      </c>
-      <c r="B3" s="372" t="s">
-        <v>499</v>
       </c>
       <c r="C3" s="372"/>
       <c r="D3" s="372"/>
@@ -18416,10 +18372,10 @@
     </row>
     <row r="4" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="369" t="s">
+        <v>499</v>
+      </c>
+      <c r="B4" s="373" t="s">
         <v>500</v>
-      </c>
-      <c r="B4" s="373" t="s">
-        <v>501</v>
       </c>
       <c r="C4" s="104"/>
       <c r="D4" s="374"/>
@@ -18428,7 +18384,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="369" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B5" s="376" t="str">
         <f aca="false">A3</f>
@@ -18442,7 +18398,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="369" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B6" s="376"/>
       <c r="C6" s="376"/>
@@ -18452,7 +18408,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="369" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B7" s="376"/>
       <c r="C7" s="376"/>
@@ -18462,7 +18418,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="369" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B8" s="376"/>
       <c r="C8" s="376"/>
@@ -18472,7 +18428,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="369" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B9" s="376"/>
       <c r="C9" s="376"/>
@@ -18482,7 +18438,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="369" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B10" s="376"/>
       <c r="C10" s="376"/>
@@ -18492,10 +18448,10 @@
     </row>
     <row r="11" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="162" t="s">
+        <v>507</v>
+      </c>
+      <c r="B11" s="377" t="s">
         <v>508</v>
-      </c>
-      <c r="B11" s="377" t="s">
-        <v>509</v>
       </c>
       <c r="C11" s="377"/>
       <c r="D11" s="377"/>
@@ -18504,7 +18460,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="162" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B12" s="378" t="n">
         <v>1</v>
@@ -18519,7 +18475,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="162" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B13" s="378" t="n">
         <v>2</v>
@@ -18534,7 +18490,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="162" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B14" s="378" t="n">
         <v>3</v>
@@ -18549,25 +18505,25 @@
     </row>
     <row r="15" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="162" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B15" s="380"/>
       <c r="C15" s="381" t="s">
+        <v>513</v>
+      </c>
+      <c r="D15" s="381" t="s">
         <v>514</v>
       </c>
-      <c r="D15" s="381" t="s">
+      <c r="E15" s="381" t="s">
         <v>515</v>
       </c>
-      <c r="E15" s="381" t="s">
+      <c r="F15" s="382" t="s">
         <v>516</v>
-      </c>
-      <c r="F15" s="382" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="162" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B16" s="383"/>
       <c r="C16" s="122" t="s">
@@ -18580,12 +18536,12 @@
         <v>61</v>
       </c>
       <c r="F16" s="122" t="s">
-        <v>289</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="162" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B17" s="378" t="n">
         <v>1</v>
@@ -18609,7 +18565,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="162" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B18" s="378" t="n">
         <v>2</v>
@@ -18633,7 +18589,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="162" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B19" s="378" t="n">
         <v>3</v>
@@ -18657,10 +18613,10 @@
     </row>
     <row r="20" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="162" t="s">
+        <v>521</v>
+      </c>
+      <c r="B20" s="385" t="s">
         <v>522</v>
-      </c>
-      <c r="B20" s="385" t="s">
-        <v>523</v>
       </c>
       <c r="C20" s="104"/>
       <c r="D20" s="374"/>
@@ -18669,7 +18625,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="162" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B21" s="376" t="str">
         <f aca="false">A23</f>
@@ -18682,7 +18638,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="162" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B22" s="376"/>
       <c r="C22" s="376"/>
@@ -18692,7 +18648,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="162" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B23" s="376"/>
       <c r="C23" s="376"/>
@@ -18702,7 +18658,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="162" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B24" s="376"/>
       <c r="C24" s="376"/>
@@ -18712,7 +18668,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="162" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B25" s="376"/>
       <c r="C25" s="376"/>
@@ -18722,7 +18678,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="162" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B26" s="376"/>
       <c r="C26" s="376"/>
@@ -18732,10 +18688,10 @@
     </row>
     <row r="27" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="162" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B27" s="377" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C27" s="377"/>
       <c r="D27" s="377"/>
@@ -18744,7 +18700,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="162" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B28" s="378" t="n">
         <v>1</v>
@@ -18759,7 +18715,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="162" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B29" s="378" t="n">
         <v>2</v>
@@ -18774,7 +18730,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="162" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B30" s="378" t="n">
         <v>3</v>
@@ -18789,25 +18745,25 @@
     </row>
     <row r="31" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="162" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B31" s="387"/>
       <c r="C31" s="381" t="s">
+        <v>513</v>
+      </c>
+      <c r="D31" s="381" t="s">
         <v>514</v>
       </c>
-      <c r="D31" s="381" t="s">
+      <c r="E31" s="381" t="s">
         <v>515</v>
       </c>
-      <c r="E31" s="381" t="s">
+      <c r="F31" s="382" t="s">
         <v>516</v>
-      </c>
-      <c r="F31" s="382" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="162" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B32" s="387"/>
       <c r="C32" s="122" t="s">
@@ -18820,12 +18776,12 @@
         <v>61</v>
       </c>
       <c r="F32" s="122" t="s">
-        <v>289</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="162" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B33" s="378" t="n">
         <v>1</v>
@@ -18849,7 +18805,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="162" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B34" s="378" t="n">
         <v>2</v>
@@ -18873,7 +18829,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="162" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B35" s="378" t="n">
         <v>3</v>
@@ -18897,10 +18853,10 @@
     </row>
     <row r="36" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="162" t="s">
+        <v>538</v>
+      </c>
+      <c r="B36" s="385" t="s">
         <v>539</v>
-      </c>
-      <c r="B36" s="385" t="s">
-        <v>540</v>
       </c>
       <c r="C36" s="388"/>
       <c r="D36" s="15"/>
@@ -18909,7 +18865,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="162" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B37" s="376" t="str">
         <f aca="false">A43</f>
@@ -18922,7 +18878,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="162" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B38" s="376"/>
       <c r="C38" s="376"/>
@@ -18932,7 +18888,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="162" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B39" s="376"/>
       <c r="C39" s="376"/>
@@ -18942,7 +18898,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="162" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B40" s="376"/>
       <c r="C40" s="376"/>
@@ -18952,7 +18908,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="162" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B41" s="376"/>
       <c r="C41" s="376"/>
@@ -18962,7 +18918,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="162" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B42" s="376"/>
       <c r="C42" s="376"/>
@@ -18972,10 +18928,10 @@
     </row>
     <row r="43" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="162" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B43" s="377" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C43" s="377"/>
       <c r="D43" s="377"/>
@@ -18984,7 +18940,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="162" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B44" s="378" t="n">
         <v>1</v>
@@ -18999,7 +18955,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="162" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B45" s="378" t="n">
         <v>2</v>
@@ -19014,7 +18970,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="162" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B46" s="378" t="n">
         <v>3</v>
@@ -19029,25 +18985,25 @@
     </row>
     <row r="47" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="162" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B47" s="387"/>
       <c r="C47" s="381" t="s">
+        <v>513</v>
+      </c>
+      <c r="D47" s="381" t="s">
         <v>514</v>
       </c>
-      <c r="D47" s="381" t="s">
+      <c r="E47" s="381" t="s">
         <v>515</v>
       </c>
-      <c r="E47" s="381" t="s">
+      <c r="F47" s="382" t="s">
         <v>516</v>
-      </c>
-      <c r="F47" s="382" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="162" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B48" s="387"/>
       <c r="C48" s="122" t="s">
@@ -19060,12 +19016,12 @@
         <v>61</v>
       </c>
       <c r="F48" s="122" t="s">
-        <v>289</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="162" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B49" s="378" t="n">
         <v>1</v>
@@ -19089,7 +19045,7 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="162" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B50" s="378" t="n">
         <v>2</v>
@@ -19113,7 +19069,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="162" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B51" s="378" t="n">
         <v>3</v>
@@ -19137,7 +19093,7 @@
     </row>
     <row r="52" customFormat="false" ht="16.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="369" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B52" s="294" t="str">
         <f aca="false">"Certifikatbeteckning: "&amp;A1&amp;", 6/8"</f>
@@ -19150,48 +19106,48 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="369" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B53" s="389"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="369" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="369" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="369" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="369" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="369" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="369" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="369" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="369" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
   </sheetData>
@@ -19345,10 +19301,10 @@
     </row>
     <row r="2" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="369" t="s">
+        <v>565</v>
+      </c>
+      <c r="B2" s="373" t="s">
         <v>566</v>
-      </c>
-      <c r="B2" s="373" t="s">
-        <v>567</v>
       </c>
       <c r="C2" s="104"/>
       <c r="D2" s="374"/>
@@ -19357,7 +19313,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="369" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B3" s="376" t="str">
         <f aca="false">A3</f>
@@ -19370,7 +19326,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="369" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B4" s="376"/>
       <c r="C4" s="376"/>
@@ -19380,7 +19336,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="369" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B5" s="376"/>
       <c r="C5" s="376"/>
@@ -19391,7 +19347,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="369" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B6" s="376"/>
       <c r="C6" s="376"/>
@@ -19402,7 +19358,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="369" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B7" s="376"/>
       <c r="C7" s="376"/>
@@ -19412,7 +19368,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="369" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B8" s="376"/>
       <c r="C8" s="376"/>
@@ -19422,7 +19378,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="369" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B9" s="376"/>
       <c r="C9" s="376"/>
@@ -19432,10 +19388,10 @@
     </row>
     <row r="10" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="162" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B10" s="390" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C10" s="390"/>
       <c r="D10" s="390"/>
@@ -19444,7 +19400,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="162" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B11" s="378" t="n">
         <v>1</v>
@@ -19459,7 +19415,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="162" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B12" s="378" t="n">
         <v>2</v>
@@ -19474,7 +19430,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="162" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B13" s="378" t="n">
         <v>3</v>
@@ -19489,25 +19445,25 @@
     </row>
     <row r="14" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="162" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B14" s="387"/>
       <c r="C14" s="381" t="s">
+        <v>513</v>
+      </c>
+      <c r="D14" s="381" t="s">
         <v>514</v>
       </c>
-      <c r="D14" s="381" t="s">
+      <c r="E14" s="381" t="s">
         <v>515</v>
       </c>
-      <c r="E14" s="381" t="s">
+      <c r="F14" s="382" t="s">
         <v>516</v>
-      </c>
-      <c r="F14" s="382" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="162" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B15" s="387"/>
       <c r="C15" s="122" t="s">
@@ -19520,12 +19476,12 @@
         <v>61</v>
       </c>
       <c r="F15" s="122" t="s">
-        <v>289</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="162" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B16" s="378" t="n">
         <v>1</v>
@@ -19549,7 +19505,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="162" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B17" s="378" t="n">
         <v>2</v>
@@ -19573,7 +19529,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="162" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B18" s="378" t="n">
         <v>3</v>
@@ -19597,10 +19553,10 @@
     </row>
     <row r="19" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="162" t="s">
+        <v>583</v>
+      </c>
+      <c r="B19" s="385" t="s">
         <v>584</v>
-      </c>
-      <c r="B19" s="385" t="s">
-        <v>585</v>
       </c>
       <c r="C19" s="388"/>
       <c r="D19" s="15"/>
@@ -19609,7 +19565,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="162" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B20" s="376" t="str">
         <f aca="false">A23</f>
@@ -19622,7 +19578,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="162" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B21" s="376"/>
       <c r="C21" s="376"/>
@@ -19632,7 +19588,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="162" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B22" s="376"/>
       <c r="C22" s="376"/>
@@ -19642,7 +19598,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="162" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B23" s="376"/>
       <c r="C23" s="376"/>
@@ -19652,7 +19608,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="162" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B24" s="376"/>
       <c r="C24" s="376"/>
@@ -19662,7 +19618,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="162" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B25" s="376"/>
       <c r="C25" s="376"/>
@@ -19672,7 +19628,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="162" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B26" s="376"/>
       <c r="C26" s="376"/>
@@ -19682,10 +19638,10 @@
     </row>
     <row r="27" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="162" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B27" s="390" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C27" s="390"/>
       <c r="D27" s="390"/>
@@ -19694,7 +19650,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="162" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B28" s="378" t="n">
         <v>1</v>
@@ -19709,7 +19665,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="162" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B29" s="378" t="n">
         <v>2</v>
@@ -19724,7 +19680,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="162" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B30" s="378" t="n">
         <v>3</v>
@@ -19739,25 +19695,25 @@
     </row>
     <row r="31" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="162" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B31" s="387"/>
       <c r="C31" s="381" t="s">
+        <v>513</v>
+      </c>
+      <c r="D31" s="381" t="s">
         <v>514</v>
       </c>
-      <c r="D31" s="381" t="s">
+      <c r="E31" s="381" t="s">
         <v>515</v>
       </c>
-      <c r="E31" s="381" t="s">
+      <c r="F31" s="382" t="s">
         <v>516</v>
-      </c>
-      <c r="F31" s="382" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="162" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B32" s="387"/>
       <c r="C32" s="122" t="s">
@@ -19770,12 +19726,12 @@
         <v>61</v>
       </c>
       <c r="F32" s="122" t="s">
-        <v>289</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="162" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B33" s="378" t="n">
         <v>1</v>
@@ -19799,7 +19755,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="162" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B34" s="378" t="n">
         <v>2</v>
@@ -19823,7 +19779,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="162" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B35" s="378" t="n">
         <v>3</v>
@@ -19847,10 +19803,10 @@
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="162" t="s">
+        <v>601</v>
+      </c>
+      <c r="B36" s="392" t="s">
         <v>602</v>
-      </c>
-      <c r="B36" s="392" t="s">
-        <v>603</v>
       </c>
       <c r="C36" s="392"/>
       <c r="D36" s="392"/>
@@ -19859,7 +19815,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="162" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B37" s="376" t="str">
         <f aca="false">A43</f>
@@ -19872,7 +19828,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="162" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B38" s="376"/>
       <c r="C38" s="376"/>
@@ -19882,7 +19838,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="162" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B39" s="376"/>
       <c r="C39" s="376"/>
@@ -19892,7 +19848,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="162" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B40" s="376"/>
       <c r="C40" s="376"/>
@@ -19902,7 +19858,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="162" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B41" s="376"/>
       <c r="C41" s="376"/>
@@ -19912,7 +19868,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="162" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B42" s="376"/>
       <c r="C42" s="376"/>
@@ -19922,7 +19878,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="162" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B43" s="376"/>
       <c r="C43" s="376"/>
@@ -19932,7 +19888,7 @@
     </row>
     <row r="44" customFormat="false" ht="19.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="162" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B44" s="376"/>
       <c r="C44" s="376"/>
@@ -19942,7 +19898,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="162" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B45" s="376"/>
       <c r="C45" s="376"/>
@@ -20000,7 +19956,7 @@
     </row>
     <row r="52" customFormat="false" ht="16.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B52" s="373" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C52" s="104"/>
       <c r="D52" s="374"/>
@@ -20018,7 +19974,7 @@
     <row r="54" customFormat="false" ht="11.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="162"/>
       <c r="B54" s="335" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C54" s="335"/>
       <c r="D54" s="335"/>
@@ -20179,8 +20135,8 @@
   </sheetPr>
   <dimension ref="A1:Q140"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B4" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B22" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B62" activeCellId="0" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20201,11 +20157,11 @@
     </row>
     <row r="2" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="162" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B2" s="395"/>
       <c r="C2" s="396" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="D2" s="396"/>
       <c r="E2" s="396"/>
@@ -20220,7 +20176,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="369" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B3" s="360"/>
       <c r="C3" s="397" t="str">
@@ -20240,7 +20196,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="369" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B4" s="360"/>
       <c r="C4" s="397"/>
@@ -20257,7 +20213,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="369" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B5" s="360"/>
       <c r="C5" s="397"/>
@@ -20274,7 +20230,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="369" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B6" s="360"/>
       <c r="C6" s="397"/>
@@ -20292,7 +20248,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="369" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B7" s="360"/>
       <c r="C7" s="397"/>
@@ -20311,7 +20267,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="369" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B8" s="360"/>
       <c r="C8" s="397"/>
@@ -20328,7 +20284,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="369" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B9" s="360"/>
       <c r="C9" s="397"/>
@@ -20346,7 +20302,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="369" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B10" s="360"/>
       <c r="C10" s="397"/>
@@ -20363,7 +20319,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="369" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B11" s="360"/>
       <c r="C11" s="397"/>
@@ -20380,7 +20336,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="369" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B12" s="360"/>
       <c r="C12" s="397"/>
@@ -20397,7 +20353,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="369" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B13" s="360"/>
       <c r="C13" s="397"/>
@@ -20414,7 +20370,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="369" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B14" s="360"/>
       <c r="C14" s="397"/>
@@ -20431,7 +20387,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="369" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B15" s="360"/>
       <c r="C15" s="397"/>
@@ -20448,7 +20404,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="369" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B16" s="360"/>
       <c r="C16" s="397"/>
@@ -20465,7 +20421,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="369" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B17" s="360"/>
       <c r="C17" s="397"/>
@@ -20482,7 +20438,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="369" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B18" s="360"/>
       <c r="C18" s="397"/>
@@ -20499,7 +20455,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="369" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B19" s="360"/>
       <c r="C19" s="397"/>
@@ -20516,7 +20472,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="369" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B20" s="360"/>
       <c r="C20" s="397"/>
@@ -20533,7 +20489,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="369" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B21" s="360"/>
       <c r="C21" s="397"/>
@@ -20550,7 +20506,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="369" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B22" s="360"/>
       <c r="C22" s="397"/>
@@ -20567,7 +20523,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="369" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B23" s="360"/>
       <c r="C23" s="397"/>
@@ -20584,7 +20540,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="369" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B24" s="360"/>
       <c r="C24" s="397"/>
@@ -20601,7 +20557,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="369" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B25" s="360"/>
       <c r="C25" s="397"/>
@@ -20618,7 +20574,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="369" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B26" s="360"/>
       <c r="C26" s="397"/>
@@ -20635,7 +20591,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="369" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B27" s="360"/>
       <c r="C27" s="397"/>
@@ -20653,7 +20609,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="369" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B28" s="360"/>
       <c r="C28" s="397"/>
@@ -20670,7 +20626,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="369" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B29" s="360"/>
       <c r="C29" s="397"/>
@@ -20687,7 +20643,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="369" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B30" s="360"/>
       <c r="C30" s="397"/>
@@ -20704,7 +20660,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="369" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B31" s="360"/>
       <c r="C31" s="397"/>
@@ -20722,7 +20678,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="369" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B32" s="360"/>
       <c r="C32" s="397"/>
@@ -20739,7 +20695,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="369" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B33" s="360"/>
       <c r="C33" s="397"/>
@@ -20756,7 +20712,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="369" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B34" s="360"/>
       <c r="C34" s="397"/>
@@ -20773,7 +20729,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="369" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B35" s="360"/>
       <c r="C35" s="397"/>
@@ -20790,7 +20746,7 @@
     </row>
     <row r="36" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="369" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B36" s="360"/>
       <c r="C36" s="397"/>
@@ -20807,7 +20763,7 @@
     </row>
     <row r="37" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="369" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B37" s="360"/>
       <c r="C37" s="397"/>
@@ -20824,7 +20780,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="369" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B38" s="360"/>
       <c r="C38" s="397"/>
@@ -20841,7 +20797,7 @@
     </row>
     <row r="39" customFormat="false" ht="24.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="369" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B39" s="360"/>
       <c r="C39" s="397"/>
@@ -20858,7 +20814,7 @@
     </row>
     <row r="40" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="369" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B40" s="360"/>
       <c r="C40" s="397"/>
@@ -20875,7 +20831,7 @@
     </row>
     <row r="41" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="369" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B41" s="360"/>
       <c r="C41" s="397"/>
@@ -20892,7 +20848,7 @@
     </row>
     <row r="42" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="369" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B42" s="360"/>
       <c r="C42" s="397"/>
@@ -20909,7 +20865,7 @@
     </row>
     <row r="43" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="369" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B43" s="360"/>
       <c r="C43" s="397"/>
@@ -20926,7 +20882,7 @@
     </row>
     <row r="44" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="369" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B44" s="360"/>
       <c r="C44" s="397"/>
@@ -20943,7 +20899,7 @@
     </row>
     <row r="45" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="369" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B45" s="360"/>
       <c r="C45" s="397"/>
@@ -20960,7 +20916,7 @@
     </row>
     <row r="46" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="369" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B46" s="360"/>
       <c r="C46" s="397"/>
@@ -20977,7 +20933,7 @@
     </row>
     <row r="47" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="369" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B47" s="360"/>
       <c r="C47" s="397"/>
@@ -20994,7 +20950,7 @@
     </row>
     <row r="48" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="369" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B48" s="360"/>
       <c r="C48" s="397"/>
@@ -21011,7 +20967,7 @@
     </row>
     <row r="49" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="369" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B49" s="360"/>
       <c r="C49" s="397"/>
@@ -21028,7 +20984,7 @@
     </row>
     <row r="50" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="369" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B50" s="360"/>
       <c r="C50" s="397"/>
@@ -21045,7 +21001,7 @@
     </row>
     <row r="51" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="369" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B51" s="360"/>
       <c r="C51" s="397"/>
@@ -21062,7 +21018,7 @@
     </row>
     <row r="52" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="369" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B52" s="360"/>
       <c r="C52" s="397"/>
@@ -21079,7 +21035,7 @@
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="369" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B53" s="360"/>
       <c r="C53" s="397"/>
@@ -21096,7 +21052,7 @@
     </row>
     <row r="54" customFormat="false" ht="7.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="369" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B54" s="360"/>
       <c r="C54" s="398"/>
@@ -21113,11 +21069,11 @@
     </row>
     <row r="55" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="369" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B55" s="400"/>
       <c r="C55" s="401" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="D55" s="401"/>
       <c r="E55" s="401"/>
@@ -21132,11 +21088,11 @@
     </row>
     <row r="56" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="369" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B56" s="402"/>
       <c r="C56" s="403" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="D56" s="403"/>
       <c r="E56" s="403"/>
@@ -21154,11 +21110,11 @@
     </row>
     <row r="57" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="369" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B57" s="402"/>
       <c r="C57" s="403" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="D57" s="403"/>
       <c r="E57" s="403"/>
@@ -21176,11 +21132,11 @@
     </row>
     <row r="58" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="369" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B58" s="402"/>
       <c r="C58" s="403" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="D58" s="403"/>
       <c r="E58" s="403"/>
@@ -21198,11 +21154,11 @@
     </row>
     <row r="59" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="369" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B59" s="402"/>
       <c r="C59" s="405" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="D59" s="405"/>
       <c r="E59" s="405"/>
@@ -21220,11 +21176,11 @@
     </row>
     <row r="60" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="369" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B60" s="402"/>
       <c r="C60" s="405" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="D60" s="405"/>
       <c r="E60" s="405"/>
@@ -21242,11 +21198,11 @@
     </row>
     <row r="61" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="369" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B61" s="406"/>
       <c r="C61" s="407" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="D61" s="407"/>
       <c r="E61" s="407"/>
@@ -21264,7 +21220,7 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="369" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B62" s="409" t="str">
         <f aca="false">"Certifikatbeteckning: "&amp;A1&amp;", 8/8"</f>
@@ -21284,7 +21240,7 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="369" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B63" s="409"/>
       <c r="C63" s="409"/>
@@ -21301,387 +21257,387 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="369" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="369" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="369" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="369" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="369" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="369" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="369" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="369" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="369" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="369" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="369" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="369" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="369" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="369" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="369" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="369" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="369" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="369" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="369" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="369" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="369" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="369" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="369" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="369" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="369" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="369" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="369" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="369" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="369" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="369" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="369" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="369" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="369" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="369" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="369" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="369" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="369" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="369" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="369" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="369" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="369" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="369" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="369" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="369" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="369" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="369" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="369" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="369" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="369" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="369" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="369" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="369" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="369" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="369" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="369" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="369" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="369" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="369" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="369" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="369" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="369" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="369" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="369" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="369" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="369" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="369" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="369" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="369" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="369" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="369" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="369" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="369" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="369" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="369" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="369" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="369" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="369" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AE-1558 Address missing translations in 2018 ET
Energiatodistuksen laatimisessa käytettyjä lähtötietoja ->
Utgångsuppgifter som används för att upprätta energicertifikat

Rakennuksen ilmatilavuus -> Byggnadens luftvolym
</commit_message>
<xml_diff>
--- a/etp-backend/src/main/resources/energiatodistus-2018-sv.xlsx
+++ b/etp-backend/src/main/resources/energiatodistus-2018-sv.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="1) etusivu" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,23 +19,23 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'1) etusivu'!$B$1:$R$51</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$58</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$59</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area" vbProcedure="false">'3) E-luvun laskennan lähtöt.'!$B$2:$G$67</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$2:$G$77</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$1:$G$78</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area" vbProcedure="false">'5) toteutunut kulutus'!$B$2:$K$55</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm.Print_Area" vbProcedure="false">'6) huomiot 1'!$B$2:$F$53</definedName>
-    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$60</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$61</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area" vbProcedure="false">'8) lisämerkintöjä'!$B$1:$M$63</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'1) etusivu'!$B$1:$R$50</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'2) E-luokka'!$B$2:$K$59</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$59</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'2) E-luokka'!$B$2:$J$58</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'3) E-luvun laskennan lähtöt.'!$B$2:$G$66</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$2:$G$76</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$1:$G$78</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$2:$G$77</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'5) toteutunut kulutus'!$B$2:$L$54</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'6) huomiot 1'!$B$2:$G$52</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'7) huomiot 2'!$B$2:$G$59</definedName>
-    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$61</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$60</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -2934,7 +2934,7 @@
     <t xml:space="preserve">[:tulokset :kuukausierittely 4 :tuotto :lampopumppu]</t>
   </si>
   <si>
-    <t xml:space="preserve">Energiatodistuksen laatimisessa käytettyjä lähtötietoja</t>
+    <t xml:space="preserve">Utgångsuppgifter som används för att upprätta energicertifikat</t>
   </si>
   <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 4 :tuotto :muulampo]</t>
@@ -2976,7 +2976,7 @@
     <t xml:space="preserve">[:tulokset :kuukausierittely 4 :kulutus :sahko]</t>
   </si>
   <si>
-    <t xml:space="preserve">Rakennuksen ilmatilavuus V, m³</t>
+    <t xml:space="preserve">Byggnadens luftvolym V, m³</t>
   </si>
   <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 4 :kulutus :lampo]</t>
@@ -7982,9 +7982,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>227520</xdr:colOff>
+      <xdr:colOff>227160</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>241920</xdr:rowOff>
+      <xdr:rowOff>241560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7998,7 +7998,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="4656960"/>
-          <a:ext cx="737640" cy="194400"/>
+          <a:ext cx="737280" cy="194040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8019,9 +8019,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>127440</xdr:colOff>
+      <xdr:colOff>127080</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>241920</xdr:rowOff>
+      <xdr:rowOff>241560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8035,7 +8035,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="4971240"/>
-          <a:ext cx="1081080" cy="194400"/>
+          <a:ext cx="1080720" cy="194040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8056,9 +8056,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>434160</xdr:colOff>
+      <xdr:colOff>433800</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>241920</xdr:rowOff>
+      <xdr:rowOff>241560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8072,7 +8072,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="5285520"/>
-          <a:ext cx="1387800" cy="194400"/>
+          <a:ext cx="1387440" cy="194040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8093,9 +8093,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>324720</xdr:colOff>
+      <xdr:colOff>324360</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>241920</xdr:rowOff>
+      <xdr:rowOff>241560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8109,7 +8109,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="5599800"/>
-          <a:ext cx="1711800" cy="194400"/>
+          <a:ext cx="1711440" cy="194040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8130,9 +8130,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>198000</xdr:colOff>
+      <xdr:colOff>197640</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>254880</xdr:rowOff>
+      <xdr:rowOff>254520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8146,7 +8146,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="5909760"/>
-          <a:ext cx="2018880" cy="207360"/>
+          <a:ext cx="2018520" cy="207000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8167,9 +8167,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>141120</xdr:colOff>
+      <xdr:colOff>140760</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>241920</xdr:rowOff>
+      <xdr:rowOff>241560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8183,7 +8183,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="6219720"/>
-          <a:ext cx="2355120" cy="194400"/>
+          <a:ext cx="2354760" cy="194040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8204,9 +8204,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>81360</xdr:colOff>
+      <xdr:colOff>81000</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>243000</xdr:rowOff>
+      <xdr:rowOff>242640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -8216,7 +8216,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3083040" y="6531480"/>
-          <a:ext cx="2667960" cy="193320"/>
+          <a:ext cx="2667600" cy="192960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8584,9 +8584,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>280800</xdr:colOff>
+      <xdr:colOff>280440</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>82080</xdr:rowOff>
+      <xdr:rowOff>81720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -8596,7 +8596,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1978200" y="78480"/>
-          <a:ext cx="6967080" cy="10488600"/>
+          <a:ext cx="6966720" cy="10488240"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -8725,8 +8725,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10374,8 +10374,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ65"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12572,8 +12572,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ94"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D37" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F45" activeCellId="0" sqref="F45"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14470,7 +14470,7 @@
   <dimension ref="A1:AMJ113"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16363,8 +16363,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F39" activeCellId="0" sqref="F39"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18107,7 +18107,7 @@
   <dimension ref="A1:AMJ61"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19089,8 +19089,8 @@
   </sheetPr>
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B55" activeCellId="0" sqref="B55"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19944,8 +19944,8 @@
   </sheetPr>
   <dimension ref="A1:Q140"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B62" activeCellId="0" sqref="B62"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>